<commit_message>
Asignación de autores mat 9 tema 11
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion11/ESCALETA_ MA_09_11_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion11/ESCALETA_ MA_09_11_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado09\guion11\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20640" windowHeight="7920"/>
   </bookViews>
@@ -18,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="246">
   <si>
     <t>Asignatura</t>
   </si>
@@ -756,6 +761,12 @@
   </si>
   <si>
     <t>CS_07_01</t>
+  </si>
+  <si>
+    <t>Magda</t>
+  </si>
+  <si>
+    <t>Alexander</t>
   </si>
 </sst>
 </file>
@@ -1005,70 +1016,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1221,6 +1172,66 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1283,7 +1294,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1318,7 +1329,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1529,2482 +1540,2488 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V19" sqref="V19"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="27" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="39" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="39" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="39" customWidth="1"/>
-    <col min="4" max="4" width="21" style="39" customWidth="1"/>
-    <col min="5" max="5" width="16" style="39" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="75" customWidth="1"/>
-    <col min="7" max="7" width="43.28515625" style="39" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="75" customWidth="1"/>
-    <col min="9" max="9" width="11" style="75" customWidth="1"/>
-    <col min="10" max="10" width="62.85546875" style="39" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" style="39" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" style="39" customWidth="1"/>
-    <col min="13" max="14" width="9.28515625" style="39" customWidth="1"/>
-    <col min="15" max="15" width="44.42578125" style="75" customWidth="1"/>
-    <col min="16" max="16" width="16.5703125" style="76" customWidth="1"/>
-    <col min="17" max="17" width="13.140625" style="75" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" style="39" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="39" customWidth="1"/>
-    <col min="20" max="20" width="21.7109375" style="39" customWidth="1"/>
-    <col min="21" max="21" width="14.5703125" style="39" customWidth="1"/>
-    <col min="22" max="256" width="9.140625" style="39" customWidth="1"/>
-    <col min="257" max="16384" width="9" style="39"/>
+    <col min="1" max="1" width="16.5703125" style="19" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="19" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="19" customWidth="1"/>
+    <col min="4" max="4" width="21" style="19" customWidth="1"/>
+    <col min="5" max="5" width="16" style="19" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="55" customWidth="1"/>
+    <col min="7" max="7" width="43.28515625" style="19" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="55" customWidth="1"/>
+    <col min="9" max="9" width="11" style="55" customWidth="1"/>
+    <col min="10" max="10" width="62.85546875" style="19" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" style="19" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" style="19" customWidth="1"/>
+    <col min="13" max="14" width="9.28515625" style="19" customWidth="1"/>
+    <col min="15" max="15" width="44.42578125" style="55" customWidth="1"/>
+    <col min="16" max="16" width="16.5703125" style="56" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" style="55" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" style="19" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="19" customWidth="1"/>
+    <col min="20" max="20" width="21.7109375" style="19" customWidth="1"/>
+    <col min="21" max="21" width="14.5703125" style="19" customWidth="1"/>
+    <col min="22" max="256" width="9.140625" style="19" customWidth="1"/>
+    <col min="257" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="15" customFormat="1" ht="27" customHeight="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:22" s="3" customFormat="1" ht="27" customHeight="1">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="74" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="64" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="64" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="66" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="10"/>
-      <c r="O1" s="11" t="s">
+      <c r="N1" s="61"/>
+      <c r="O1" s="69" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="P1" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="Q1" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="R1" s="71" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="S1" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="14" t="s">
+      <c r="T1" s="68" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="U1" s="58" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="15" customFormat="1" ht="27" customHeight="1" thickBot="1">
-      <c r="A2" s="16"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="23" t="s">
+    <row r="2" spans="1:22" s="3" customFormat="1" ht="27" customHeight="1" thickBot="1">
+      <c r="A2" s="63"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="N2" s="23" t="s">
+      <c r="N2" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="12"/>
-    </row>
-    <row r="3" spans="1:21" ht="27" customHeight="1" thickTop="1">
-      <c r="A3" s="25" t="s">
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="58"/>
+      <c r="R2" s="71"/>
+      <c r="S2" s="58"/>
+      <c r="T2" s="68"/>
+      <c r="U2" s="58"/>
+    </row>
+    <row r="3" spans="1:22" ht="27" customHeight="1" thickTop="1">
+      <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="E3" s="26"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="29" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="H3" s="30">
+      <c r="H3" s="10">
         <v>1</v>
       </c>
-      <c r="I3" s="30" t="s">
+      <c r="I3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="31" t="s">
+      <c r="J3" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="K3" s="32" t="s">
+      <c r="K3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="29" t="s">
+      <c r="L3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="34" t="s">
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="P3" s="35" t="s">
+      <c r="P3" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="Q3" s="36">
+      <c r="Q3" s="16">
         <v>9</v>
       </c>
-      <c r="R3" s="37" t="s">
+      <c r="R3" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="S3" s="36" t="s">
+      <c r="S3" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="T3" s="38" t="s">
+      <c r="T3" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="U3" s="36" t="s">
+      <c r="U3" s="16" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="27" customHeight="1">
-      <c r="A4" s="25" t="s">
+    <row r="4" spans="1:22" ht="27" customHeight="1">
+      <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="E4" s="40"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="42" t="s">
+      <c r="E4" s="20"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="H4" s="30">
+      <c r="H4" s="10">
         <v>2</v>
       </c>
-      <c r="I4" s="43" t="s">
+      <c r="I4" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="44" t="s">
+      <c r="J4" s="24" t="s">
         <v>164</v>
       </c>
-      <c r="K4" s="45" t="s">
+      <c r="K4" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="46" t="s">
+      <c r="L4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47" t="s">
+      <c r="M4" s="27"/>
+      <c r="N4" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="O4" s="41" t="s">
+      <c r="O4" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="P4" s="35" t="s">
+      <c r="P4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="36">
+      <c r="Q4" s="16">
         <v>6</v>
       </c>
-      <c r="R4" s="37" t="s">
+      <c r="R4" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="S4" s="36" t="s">
+      <c r="S4" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="T4" s="38" t="s">
+      <c r="T4" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="U4" s="36" t="s">
+      <c r="U4" s="16" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="27" customHeight="1">
-      <c r="A5" s="25" t="s">
+    <row r="5" spans="1:22" ht="27" customHeight="1">
+      <c r="A5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="E5" s="40"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="42" t="s">
+      <c r="E5" s="20"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="22" t="s">
         <v>190</v>
       </c>
-      <c r="H5" s="30">
+      <c r="H5" s="10">
         <v>3</v>
       </c>
-      <c r="I5" s="43" t="s">
+      <c r="I5" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="44" t="s">
+      <c r="J5" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="K5" s="45" t="s">
+      <c r="K5" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="46" t="s">
+      <c r="L5" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="M5" s="47"/>
-      <c r="N5" s="47" t="s">
+      <c r="M5" s="27"/>
+      <c r="N5" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="O5" s="41" t="s">
+      <c r="O5" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="P5" s="35" t="s">
+      <c r="P5" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="Q5" s="36">
+      <c r="Q5" s="16">
         <v>6</v>
       </c>
-      <c r="R5" s="37" t="s">
+      <c r="R5" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="S5" s="36" t="s">
+      <c r="S5" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="T5" s="38" t="s">
+      <c r="T5" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="U5" s="36" t="s">
+      <c r="U5" s="16" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="27" customHeight="1">
-      <c r="A6" s="25" t="s">
+    <row r="6" spans="1:22" ht="27" customHeight="1">
+      <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="E6" s="40"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="42" t="s">
+      <c r="E6" s="20"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="22" t="s">
         <v>191</v>
       </c>
-      <c r="H6" s="30">
+      <c r="H6" s="10">
         <v>4</v>
       </c>
-      <c r="I6" s="43" t="s">
+      <c r="I6" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="44" t="s">
+      <c r="J6" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="K6" s="45" t="s">
+      <c r="K6" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="L6" s="46" t="s">
+      <c r="L6" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="M6" s="47"/>
-      <c r="N6" s="47" t="s">
+      <c r="M6" s="27"/>
+      <c r="N6" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="O6" s="41" t="s">
+      <c r="O6" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="P6" s="35" t="s">
+      <c r="P6" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="Q6" s="36">
+      <c r="Q6" s="16">
         <v>6</v>
       </c>
-      <c r="R6" s="37" t="s">
+      <c r="R6" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="S6" s="36" t="s">
+      <c r="S6" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="T6" s="38" t="s">
+      <c r="T6" s="18" t="s">
         <v>168</v>
       </c>
-      <c r="U6" s="36" t="s">
+      <c r="U6" s="16" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="27" customHeight="1">
-      <c r="A7" s="25" t="s">
+    <row r="7" spans="1:22" ht="27" customHeight="1">
+      <c r="A7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="E7" s="40"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="42" t="s">
+      <c r="E7" s="20"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="22" t="s">
         <v>195</v>
       </c>
-      <c r="H7" s="30">
+      <c r="H7" s="10">
         <v>5</v>
       </c>
-      <c r="I7" s="43" t="s">
+      <c r="I7" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="44" t="s">
+      <c r="J7" s="24" t="s">
         <v>235</v>
       </c>
-      <c r="K7" s="45" t="s">
+      <c r="K7" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="L7" s="46" t="s">
+      <c r="L7" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="47"/>
-      <c r="N7" s="47" t="s">
+      <c r="M7" s="27"/>
+      <c r="N7" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="O7" s="41" t="s">
+      <c r="O7" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="P7" s="35" t="s">
+      <c r="P7" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="Q7" s="36">
+      <c r="Q7" s="16">
         <v>6</v>
       </c>
-      <c r="R7" s="37" t="s">
+      <c r="R7" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="S7" s="36" t="s">
+      <c r="S7" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="T7" s="38" t="s">
+      <c r="T7" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="U7" s="36" t="s">
+      <c r="U7" s="16" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="27" customHeight="1">
-      <c r="A8" s="25" t="s">
+    <row r="8" spans="1:22" ht="27" customHeight="1">
+      <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="D8" s="49" t="s">
+      <c r="D8" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="E8" s="40" t="s">
+      <c r="E8" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="F8" s="41"/>
-      <c r="G8" s="42" t="s">
+      <c r="F8" s="21"/>
+      <c r="G8" s="22" t="s">
         <v>197</v>
       </c>
-      <c r="H8" s="30">
+      <c r="H8" s="10">
         <v>6</v>
       </c>
-      <c r="I8" s="43" t="s">
+      <c r="I8" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="44" t="s">
+      <c r="J8" s="24" t="s">
         <v>236</v>
       </c>
-      <c r="K8" s="45" t="s">
+      <c r="K8" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="46" t="s">
+      <c r="L8" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="M8" s="47"/>
-      <c r="N8" s="47" t="s">
+      <c r="M8" s="27"/>
+      <c r="N8" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="O8" s="41" t="s">
+      <c r="O8" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="P8" s="35" t="s">
+      <c r="P8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="Q8" s="36">
+      <c r="Q8" s="16">
         <v>6</v>
       </c>
-      <c r="R8" s="37" t="s">
+      <c r="R8" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="S8" s="36" t="s">
+      <c r="S8" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="T8" s="38" t="s">
+      <c r="T8" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="U8" s="36" t="s">
+      <c r="U8" s="16" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="27" customHeight="1">
-      <c r="A9" s="25" t="s">
+    <row r="9" spans="1:22" ht="27" customHeight="1">
+      <c r="A9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D9" s="50" t="s">
+      <c r="D9" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="E9" s="40"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="42" t="s">
+      <c r="E9" s="20"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="22" t="s">
         <v>198</v>
       </c>
-      <c r="H9" s="30">
+      <c r="H9" s="10">
         <v>7</v>
       </c>
-      <c r="I9" s="43" t="s">
+      <c r="I9" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="44" t="s">
+      <c r="J9" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="K9" s="45" t="s">
+      <c r="K9" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="46" t="s">
+      <c r="L9" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="M9" s="47" t="s">
+      <c r="M9" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="N9" s="47"/>
-      <c r="O9" s="41" t="s">
+      <c r="N9" s="27"/>
+      <c r="O9" s="21" t="s">
         <v>199</v>
       </c>
-      <c r="P9" s="35" t="s">
+      <c r="P9" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="Q9" s="36">
+      <c r="Q9" s="16">
         <v>6</v>
       </c>
-      <c r="R9" s="37" t="s">
+      <c r="R9" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="S9" s="36" t="s">
+      <c r="S9" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="T9" s="38" t="s">
+      <c r="T9" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="U9" s="36" t="s">
+      <c r="U9" s="16" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" ht="27" customHeight="1">
-      <c r="A10" s="25" t="s">
+      <c r="V9" s="19" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="27" customHeight="1">
+      <c r="A10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D10" s="50" t="s">
+      <c r="D10" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="E10" s="40"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="42" t="s">
+      <c r="E10" s="20"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="22" t="s">
         <v>201</v>
       </c>
-      <c r="H10" s="30">
+      <c r="H10" s="10">
         <v>8</v>
       </c>
-      <c r="I10" s="43" t="s">
+      <c r="I10" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="44" t="s">
+      <c r="J10" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="K10" s="45" t="s">
+      <c r="K10" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="46" t="s">
+      <c r="L10" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="M10" s="47"/>
-      <c r="N10" s="47" t="s">
+      <c r="M10" s="27"/>
+      <c r="N10" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="O10" s="41" t="s">
+      <c r="O10" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="P10" s="35" t="s">
+      <c r="P10" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="Q10" s="36">
+      <c r="Q10" s="16">
         <v>6</v>
       </c>
-      <c r="R10" s="37" t="s">
+      <c r="R10" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="S10" s="36" t="s">
+      <c r="S10" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="T10" s="38" t="s">
+      <c r="T10" s="18" t="s">
         <v>169</v>
       </c>
-      <c r="U10" s="36" t="s">
+      <c r="U10" s="16" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="27" customHeight="1">
-      <c r="A11" s="25" t="s">
+    <row r="11" spans="1:22" ht="27" customHeight="1">
+      <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D11" s="50" t="s">
+      <c r="D11" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="E11" s="40" t="s">
+      <c r="E11" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="F11" s="41"/>
-      <c r="G11" s="42" t="s">
+      <c r="F11" s="21"/>
+      <c r="G11" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="H11" s="30">
+      <c r="H11" s="10">
         <v>9</v>
       </c>
-      <c r="I11" s="43" t="s">
+      <c r="I11" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="44" t="s">
+      <c r="J11" s="24" t="s">
         <v>204</v>
       </c>
-      <c r="K11" s="45" t="s">
+      <c r="K11" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="L11" s="46" t="s">
+      <c r="L11" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="M11" s="47"/>
-      <c r="N11" s="47" t="s">
+      <c r="M11" s="27"/>
+      <c r="N11" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="O11" s="41" t="s">
+      <c r="O11" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="P11" s="35" t="s">
+      <c r="P11" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="51">
+      <c r="Q11" s="31">
         <v>6</v>
       </c>
-      <c r="R11" s="37" t="s">
+      <c r="R11" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="S11" s="36" t="s">
+      <c r="S11" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="T11" s="38" t="s">
+      <c r="T11" s="18" t="s">
         <v>178</v>
       </c>
-      <c r="U11" s="36" t="s">
+      <c r="U11" s="16" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="27" customHeight="1">
-      <c r="A12" s="25" t="s">
+    <row r="12" spans="1:22" ht="27" customHeight="1">
+      <c r="A12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D12" s="50" t="s">
+      <c r="D12" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="E12" s="40"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="42" t="s">
+      <c r="E12" s="20"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="H12" s="30">
+      <c r="H12" s="10">
         <v>10</v>
       </c>
-      <c r="I12" s="43" t="s">
+      <c r="I12" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="J12" s="44" t="s">
+      <c r="J12" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="K12" s="45" t="s">
+      <c r="K12" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="L12" s="46" t="s">
+      <c r="L12" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="M12" s="47" t="s">
+      <c r="M12" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="N12" s="47"/>
-      <c r="O12" s="41" t="s">
+      <c r="N12" s="27"/>
+      <c r="O12" s="21" t="s">
         <v>205</v>
       </c>
-      <c r="P12" s="35" t="s">
+      <c r="P12" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="Q12" s="51">
+      <c r="Q12" s="31">
         <v>6</v>
       </c>
-      <c r="R12" s="52" t="s">
+      <c r="R12" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="S12" s="53" t="s">
+      <c r="S12" s="33" t="s">
         <v>225</v>
       </c>
-      <c r="T12" s="54" t="s">
+      <c r="T12" s="34" t="s">
         <v>226</v>
       </c>
-      <c r="U12" s="55" t="s">
+      <c r="U12" s="35" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" ht="27" customHeight="1">
-      <c r="A13" s="25" t="s">
+      <c r="V12" s="19" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="27" customHeight="1">
+      <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D13" s="50" t="s">
+      <c r="D13" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="E13" s="40"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="42" t="s">
+      <c r="E13" s="20"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="22" t="s">
         <v>206</v>
       </c>
-      <c r="H13" s="30">
+      <c r="H13" s="10">
         <v>11</v>
       </c>
-      <c r="I13" s="43" t="s">
+      <c r="I13" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="J13" s="44" t="s">
+      <c r="J13" s="24" t="s">
         <v>207</v>
       </c>
-      <c r="K13" s="45" t="s">
+      <c r="K13" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="L13" s="46" t="s">
+      <c r="L13" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="M13" s="47"/>
-      <c r="N13" s="47" t="s">
+      <c r="M13" s="27"/>
+      <c r="N13" s="27" t="s">
         <v>160</v>
       </c>
-      <c r="O13" s="41" t="s">
+      <c r="O13" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="P13" s="35" t="s">
+      <c r="P13" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="Q13" s="36">
+      <c r="Q13" s="16">
         <v>6</v>
       </c>
-      <c r="R13" s="37" t="s">
+      <c r="R13" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="S13" s="36" t="s">
+      <c r="S13" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="T13" s="38" t="s">
+      <c r="T13" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="U13" s="36" t="s">
+      <c r="U13" s="16" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="27" customHeight="1">
-      <c r="A14" s="25" t="s">
+    <row r="14" spans="1:22" ht="27" customHeight="1">
+      <c r="A14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D14" s="50" t="s">
+      <c r="D14" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="E14" s="40"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="42" t="s">
+      <c r="E14" s="20"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="22" t="s">
         <v>216</v>
       </c>
-      <c r="H14" s="30">
+      <c r="H14" s="10">
         <v>12</v>
       </c>
-      <c r="I14" s="43" t="s">
+      <c r="I14" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="J14" s="44" t="s">
+      <c r="J14" s="24" t="s">
         <v>209</v>
       </c>
-      <c r="K14" s="45" t="s">
+      <c r="K14" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="46" t="s">
+      <c r="L14" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="M14" s="47"/>
-      <c r="N14" s="47" t="s">
+      <c r="M14" s="27"/>
+      <c r="N14" s="27" t="s">
         <v>161</v>
       </c>
-      <c r="O14" s="41" t="s">
+      <c r="O14" s="21" t="s">
         <v>210</v>
       </c>
-      <c r="P14" s="35" t="s">
+      <c r="P14" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="Q14" s="36">
+      <c r="Q14" s="16">
         <v>6</v>
       </c>
-      <c r="R14" s="37" t="s">
+      <c r="R14" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="S14" s="36" t="s">
+      <c r="S14" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="T14" s="38" t="s">
+      <c r="T14" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="U14" s="36" t="s">
+      <c r="U14" s="16" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="27" customHeight="1">
-      <c r="A15" s="25" t="s">
+    <row r="15" spans="1:22" ht="27" customHeight="1">
+      <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D15" s="57" t="s">
+      <c r="D15" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="E15" s="58" t="s">
+      <c r="E15" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="F15" s="41"/>
-      <c r="G15" s="42" t="s">
+      <c r="F15" s="21"/>
+      <c r="G15" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="H15" s="30">
+      <c r="H15" s="10">
         <v>13</v>
       </c>
-      <c r="I15" s="43" t="s">
+      <c r="I15" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="J15" s="44" t="s">
+      <c r="J15" s="24" t="s">
         <v>212</v>
       </c>
-      <c r="K15" s="45" t="s">
+      <c r="K15" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="L15" s="59" t="s">
+      <c r="L15" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="M15" s="47"/>
-      <c r="N15" s="47" t="s">
+      <c r="M15" s="27"/>
+      <c r="N15" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="O15" s="41" t="s">
+      <c r="O15" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="P15" s="35" t="s">
+      <c r="P15" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="Q15" s="51">
+      <c r="Q15" s="31">
         <v>6</v>
       </c>
-      <c r="R15" s="37" t="s">
+      <c r="R15" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="S15" s="36" t="s">
+      <c r="S15" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="T15" s="38" t="s">
+      <c r="T15" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="U15" s="36" t="s">
+      <c r="U15" s="16" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="16" spans="1:21" s="65" customFormat="1" ht="27" customHeight="1">
-      <c r="A16" s="25" t="s">
+    <row r="16" spans="1:22" s="45" customFormat="1" ht="27" customHeight="1">
+      <c r="A16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="C16" s="48" t="s">
+      <c r="C16" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="D16" s="57" t="s">
+      <c r="D16" s="37" t="s">
         <v>228</v>
       </c>
-      <c r="E16" s="58"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="60" t="s">
+      <c r="E16" s="38"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="40" t="s">
         <v>217</v>
       </c>
-      <c r="H16" s="30">
+      <c r="H16" s="10">
         <v>14</v>
       </c>
-      <c r="I16" s="43" t="s">
+      <c r="I16" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="61" t="s">
+      <c r="J16" s="41" t="s">
         <v>214</v>
       </c>
-      <c r="K16" s="62" t="s">
+      <c r="K16" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="L16" s="59" t="s">
+      <c r="L16" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="M16" s="63"/>
-      <c r="N16" s="63"/>
-      <c r="O16" s="41"/>
-      <c r="P16" s="35" t="s">
+      <c r="M16" s="43"/>
+      <c r="N16" s="43"/>
+      <c r="O16" s="21"/>
+      <c r="P16" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="Q16" s="55">
+      <c r="Q16" s="35">
         <v>9</v>
       </c>
-      <c r="R16" s="52" t="s">
+      <c r="R16" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="S16" s="55" t="s">
+      <c r="S16" s="35" t="s">
         <v>229</v>
       </c>
-      <c r="T16" s="64" t="s">
+      <c r="T16" s="44" t="s">
         <v>230</v>
       </c>
-      <c r="U16" s="55" t="s">
+      <c r="U16" s="35" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="17" spans="1:22" s="65" customFormat="1" ht="27" customHeight="1">
-      <c r="A17" s="25" t="s">
+    <row r="17" spans="1:22" s="45" customFormat="1" ht="27" customHeight="1">
+      <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="56" t="s">
+      <c r="B17" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="C17" s="48" t="s">
+      <c r="C17" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="D17" s="57" t="s">
+      <c r="D17" s="37" t="s">
         <v>228</v>
       </c>
-      <c r="E17" s="58"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="60" t="s">
+      <c r="E17" s="38"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="40" t="s">
         <v>215</v>
       </c>
-      <c r="H17" s="30">
+      <c r="H17" s="10">
         <v>15</v>
       </c>
-      <c r="I17" s="43" t="s">
+      <c r="I17" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="J17" s="61" t="s">
+      <c r="J17" s="41" t="s">
         <v>187</v>
       </c>
-      <c r="K17" s="62" t="s">
+      <c r="K17" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="L17" s="59" t="s">
+      <c r="L17" s="39" t="s">
         <v>155</v>
       </c>
-      <c r="M17" s="63"/>
-      <c r="N17" s="63"/>
-      <c r="O17" s="77" t="s">
+      <c r="M17" s="43"/>
+      <c r="N17" s="43"/>
+      <c r="O17" s="57" t="s">
         <v>232</v>
       </c>
-      <c r="P17" s="66" t="s">
+      <c r="P17" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="Q17" s="51">
+      <c r="Q17" s="31">
         <v>7</v>
       </c>
-      <c r="R17" s="37" t="s">
+      <c r="R17" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="S17" s="51" t="s">
+      <c r="S17" s="31" t="s">
         <v>241</v>
       </c>
-      <c r="T17" s="67" t="s">
+      <c r="T17" s="47" t="s">
         <v>242</v>
       </c>
-      <c r="U17" s="51" t="s">
+      <c r="U17" s="31" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="18" spans="1:22" s="65" customFormat="1" ht="27" customHeight="1">
-      <c r="A18" s="25" t="s">
+    <row r="18" spans="1:22" s="45" customFormat="1" ht="27" customHeight="1">
+      <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="56" t="s">
+      <c r="B18" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="C18" s="48" t="s">
+      <c r="C18" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="D18" s="57" t="s">
+      <c r="D18" s="37" t="s">
         <v>228</v>
       </c>
-      <c r="E18" s="58" t="s">
+      <c r="E18" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="F18" s="41"/>
-      <c r="G18" s="60" t="s">
+      <c r="F18" s="21"/>
+      <c r="G18" s="40" t="s">
         <v>218</v>
       </c>
-      <c r="H18" s="30">
+      <c r="H18" s="10">
         <v>16</v>
       </c>
-      <c r="I18" s="43" t="s">
+      <c r="I18" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="J18" s="61" t="s">
+      <c r="J18" s="41" t="s">
         <v>186</v>
       </c>
-      <c r="K18" s="62" t="s">
+      <c r="K18" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="L18" s="59" t="s">
+      <c r="L18" s="39" t="s">
         <v>156</v>
       </c>
-      <c r="M18" s="63"/>
-      <c r="N18" s="63" t="s">
+      <c r="M18" s="43"/>
+      <c r="N18" s="43" t="s">
         <v>163</v>
       </c>
-      <c r="O18" s="41" t="s">
+      <c r="O18" s="21" t="s">
         <v>238</v>
       </c>
-      <c r="P18" s="66" t="s">
+      <c r="P18" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="Q18" s="51">
+      <c r="Q18" s="31">
         <v>6</v>
       </c>
-      <c r="R18" s="37" t="s">
+      <c r="R18" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="S18" s="36" t="s">
+      <c r="S18" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="T18" s="38" t="s">
+      <c r="T18" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="U18" s="36" t="s">
+      <c r="U18" s="16" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:22" ht="27" customHeight="1">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C19" s="48" t="s">
+      <c r="C19" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="D19" s="57" t="s">
+      <c r="D19" s="37" t="s">
         <v>127</v>
       </c>
-      <c r="E19" s="58"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="60" t="s">
+      <c r="E19" s="38"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="40" t="s">
         <v>219</v>
       </c>
-      <c r="H19" s="30">
+      <c r="H19" s="10">
         <v>17</v>
       </c>
-      <c r="I19" s="43" t="s">
+      <c r="I19" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="61" t="s">
+      <c r="J19" s="41" t="s">
         <v>233</v>
       </c>
-      <c r="K19" s="62" t="s">
+      <c r="K19" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="L19" s="59" t="s">
+      <c r="L19" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="M19" s="47"/>
-      <c r="N19" s="47" t="s">
+      <c r="M19" s="27"/>
+      <c r="N19" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="O19" s="41" t="s">
+      <c r="O19" s="21" t="s">
         <v>220</v>
       </c>
-      <c r="P19" s="66" t="s">
+      <c r="P19" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="Q19" s="55">
+      <c r="Q19" s="35">
         <v>6</v>
       </c>
-      <c r="R19" s="52" t="s">
+      <c r="R19" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="S19" s="55" t="s">
+      <c r="S19" s="35" t="s">
         <v>165</v>
       </c>
-      <c r="T19" s="54" t="s">
+      <c r="T19" s="34" t="s">
         <v>172</v>
       </c>
-      <c r="U19" s="55" t="s">
+      <c r="U19" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="V19" s="37"/>
+      <c r="V19" s="17"/>
     </row>
     <row r="20" spans="1:22" ht="27" customHeight="1">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D20" s="50" t="s">
+      <c r="D20" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="E20" s="40"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="60" t="s">
+      <c r="E20" s="20"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="H20" s="30">
+      <c r="H20" s="10">
         <v>18</v>
       </c>
-      <c r="I20" s="43" t="s">
+      <c r="I20" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="J20" s="68" t="s">
+      <c r="J20" s="48" t="s">
         <v>221</v>
       </c>
-      <c r="K20" s="62" t="s">
+      <c r="K20" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="L20" s="46" t="s">
+      <c r="L20" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="M20" s="47"/>
-      <c r="N20" s="47"/>
-      <c r="O20" s="41"/>
-      <c r="P20" s="66" t="s">
+      <c r="M20" s="27"/>
+      <c r="N20" s="27"/>
+      <c r="O20" s="21"/>
+      <c r="P20" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="Q20" s="36"/>
-      <c r="R20" s="37"/>
-      <c r="S20" s="36"/>
-      <c r="T20" s="38"/>
-      <c r="U20" s="36"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="17"/>
+      <c r="S20" s="16"/>
+      <c r="T20" s="18"/>
+      <c r="U20" s="16"/>
     </row>
     <row r="21" spans="1:22" ht="27" customHeight="1">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D21" s="50" t="s">
+      <c r="D21" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="E21" s="40"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="60" t="s">
+      <c r="E21" s="20"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="H21" s="30">
+      <c r="H21" s="10">
         <v>19</v>
       </c>
-      <c r="I21" s="43" t="s">
+      <c r="I21" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="J21" s="44" t="s">
+      <c r="J21" s="24" t="s">
         <v>223</v>
       </c>
-      <c r="K21" s="45" t="s">
+      <c r="K21" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="L21" s="46" t="s">
+      <c r="L21" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="M21" s="47"/>
-      <c r="N21" s="47" t="s">
+      <c r="M21" s="27"/>
+      <c r="N21" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="O21" s="41" t="s">
+      <c r="O21" s="21" t="s">
         <v>237</v>
       </c>
-      <c r="P21" s="66" t="s">
+      <c r="P21" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="Q21" s="36">
+      <c r="Q21" s="16">
         <v>6</v>
       </c>
-      <c r="R21" s="37" t="s">
+      <c r="R21" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="S21" s="36" t="s">
+      <c r="S21" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="T21" s="38" t="s">
+      <c r="T21" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="U21" s="36" t="s">
+      <c r="U21" s="16" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:22" ht="27" customHeight="1">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C22" s="27" t="s">
+      <c r="C22" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D22" s="50" t="s">
+      <c r="D22" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="E22" s="50"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="42" t="s">
+      <c r="E22" s="30"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="22" t="s">
         <v>222</v>
       </c>
-      <c r="H22" s="30">
+      <c r="H22" s="10">
         <v>20</v>
       </c>
-      <c r="I22" s="43" t="s">
+      <c r="I22" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="68" t="s">
+      <c r="J22" s="48" t="s">
         <v>234</v>
       </c>
-      <c r="K22" s="45" t="s">
+      <c r="K22" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="L22" s="46" t="s">
+      <c r="L22" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="M22" s="47"/>
-      <c r="N22" s="47" t="s">
+      <c r="M22" s="27"/>
+      <c r="N22" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="O22" s="41" t="s">
+      <c r="O22" s="21" t="s">
         <v>237</v>
       </c>
-      <c r="P22" s="66" t="s">
+      <c r="P22" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="Q22" s="36">
+      <c r="Q22" s="16">
         <v>6</v>
       </c>
-      <c r="R22" s="37" t="s">
+      <c r="R22" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="S22" s="36" t="s">
+      <c r="S22" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="T22" s="38" t="s">
+      <c r="T22" s="18" t="s">
         <v>182</v>
       </c>
-      <c r="U22" s="36" t="s">
+      <c r="U22" s="16" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:22" ht="27" customHeight="1">
-      <c r="A23" s="69"/>
-      <c r="B23" s="40"/>
-      <c r="C23" s="70"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="71"/>
-      <c r="J23" s="44"/>
-      <c r="K23" s="45"/>
-      <c r="L23" s="46"/>
-      <c r="M23" s="47"/>
-      <c r="N23" s="47"/>
-      <c r="O23" s="41"/>
-      <c r="P23" s="66"/>
-      <c r="Q23" s="36"/>
-      <c r="R23" s="37"/>
-      <c r="S23" s="36"/>
-      <c r="T23" s="38"/>
-      <c r="U23" s="36"/>
+      <c r="A23" s="49"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="25"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="27"/>
+      <c r="N23" s="27"/>
+      <c r="O23" s="21"/>
+      <c r="P23" s="46"/>
+      <c r="Q23" s="16"/>
+      <c r="R23" s="17"/>
+      <c r="S23" s="16"/>
+      <c r="T23" s="18"/>
+      <c r="U23" s="16"/>
     </row>
     <row r="24" spans="1:22" ht="27" customHeight="1">
-      <c r="A24" s="69"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="70"/>
-      <c r="D24" s="50"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="71"/>
-      <c r="J24" s="44"/>
-      <c r="K24" s="45"/>
-      <c r="L24" s="46"/>
-      <c r="M24" s="47"/>
-      <c r="N24" s="47"/>
-      <c r="O24" s="41"/>
-      <c r="P24" s="66"/>
-      <c r="Q24" s="36"/>
-      <c r="R24" s="37"/>
-      <c r="S24" s="36"/>
-      <c r="T24" s="38"/>
-      <c r="U24" s="36"/>
+      <c r="A24" s="49"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="27"/>
+      <c r="N24" s="27"/>
+      <c r="O24" s="21"/>
+      <c r="P24" s="46"/>
+      <c r="Q24" s="16"/>
+      <c r="R24" s="17"/>
+      <c r="S24" s="16"/>
+      <c r="T24" s="18"/>
+      <c r="U24" s="16"/>
     </row>
     <row r="25" spans="1:22" ht="27" customHeight="1">
-      <c r="A25" s="69"/>
-      <c r="B25" s="40"/>
-      <c r="C25" s="70"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="41"/>
-      <c r="I25" s="71"/>
-      <c r="J25" s="44"/>
-      <c r="K25" s="45"/>
-      <c r="L25" s="46"/>
-      <c r="M25" s="47"/>
-      <c r="N25" s="47"/>
-      <c r="O25" s="41"/>
-      <c r="P25" s="66"/>
-      <c r="Q25" s="36"/>
-      <c r="R25" s="37"/>
-      <c r="S25" s="36"/>
-      <c r="T25" s="38"/>
-      <c r="U25" s="36"/>
+      <c r="A25" s="49"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="51"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="27"/>
+      <c r="N25" s="27"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="46"/>
+      <c r="Q25" s="16"/>
+      <c r="R25" s="17"/>
+      <c r="S25" s="16"/>
+      <c r="T25" s="18"/>
+      <c r="U25" s="16"/>
     </row>
     <row r="26" spans="1:22" ht="27" customHeight="1">
-      <c r="A26" s="72"/>
-      <c r="B26" s="73"/>
-      <c r="C26" s="73"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="73"/>
-      <c r="F26" s="73"/>
-      <c r="G26" s="73"/>
-      <c r="H26" s="73"/>
-      <c r="I26" s="72"/>
-      <c r="J26" s="73"/>
-      <c r="K26" s="72"/>
-      <c r="L26" s="72"/>
-      <c r="M26" s="72"/>
-      <c r="N26" s="72"/>
-      <c r="O26" s="73"/>
-      <c r="P26" s="74"/>
-      <c r="Q26" s="73"/>
-      <c r="R26" s="73"/>
-      <c r="S26" s="73"/>
-      <c r="T26" s="73"/>
-      <c r="U26" s="73"/>
-      <c r="V26" s="65"/>
+      <c r="A26" s="52"/>
+      <c r="B26" s="53"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="52"/>
+      <c r="J26" s="53"/>
+      <c r="K26" s="52"/>
+      <c r="L26" s="52"/>
+      <c r="M26" s="52"/>
+      <c r="N26" s="52"/>
+      <c r="O26" s="53"/>
+      <c r="P26" s="54"/>
+      <c r="Q26" s="53"/>
+      <c r="R26" s="53"/>
+      <c r="S26" s="53"/>
+      <c r="T26" s="53"/>
+      <c r="U26" s="53"/>
+      <c r="V26" s="45"/>
     </row>
     <row r="27" spans="1:22" ht="27" customHeight="1">
-      <c r="A27" s="72"/>
-      <c r="B27" s="73"/>
-      <c r="C27" s="73"/>
-      <c r="D27" s="73"/>
-      <c r="E27" s="73"/>
-      <c r="F27" s="73"/>
-      <c r="G27" s="73"/>
-      <c r="H27" s="73"/>
-      <c r="I27" s="72"/>
-      <c r="J27" s="73"/>
-      <c r="K27" s="72"/>
-      <c r="L27" s="72"/>
-      <c r="M27" s="72"/>
-      <c r="N27" s="72"/>
-      <c r="O27" s="73"/>
-      <c r="P27" s="74"/>
-      <c r="Q27" s="73"/>
-      <c r="R27" s="73"/>
-      <c r="S27" s="73"/>
-      <c r="T27" s="73"/>
-      <c r="U27" s="73"/>
-      <c r="V27" s="65"/>
+      <c r="A27" s="52"/>
+      <c r="B27" s="53"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="53"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="53"/>
+      <c r="K27" s="52"/>
+      <c r="L27" s="52"/>
+      <c r="M27" s="52"/>
+      <c r="N27" s="52"/>
+      <c r="O27" s="53"/>
+      <c r="P27" s="54"/>
+      <c r="Q27" s="53"/>
+      <c r="R27" s="53"/>
+      <c r="S27" s="53"/>
+      <c r="T27" s="53"/>
+      <c r="U27" s="53"/>
+      <c r="V27" s="45"/>
     </row>
     <row r="28" spans="1:22" ht="27" customHeight="1">
-      <c r="A28" s="72"/>
-      <c r="B28" s="73"/>
-      <c r="C28" s="73"/>
-      <c r="D28" s="73"/>
-      <c r="E28" s="73"/>
-      <c r="F28" s="73"/>
-      <c r="G28" s="73"/>
-      <c r="H28" s="73"/>
-      <c r="I28" s="72"/>
-      <c r="J28" s="73"/>
-      <c r="K28" s="72"/>
-      <c r="L28" s="72"/>
-      <c r="M28" s="72"/>
-      <c r="N28" s="72"/>
-      <c r="O28" s="73"/>
-      <c r="P28" s="74"/>
-      <c r="Q28" s="73"/>
-      <c r="R28" s="73"/>
-      <c r="S28" s="73"/>
-      <c r="T28" s="73"/>
-      <c r="U28" s="73"/>
-      <c r="V28" s="65"/>
+      <c r="A28" s="52"/>
+      <c r="B28" s="53"/>
+      <c r="C28" s="53"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="53"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="52"/>
+      <c r="J28" s="53"/>
+      <c r="K28" s="52"/>
+      <c r="L28" s="52"/>
+      <c r="M28" s="52"/>
+      <c r="N28" s="52"/>
+      <c r="O28" s="53"/>
+      <c r="P28" s="54"/>
+      <c r="Q28" s="53"/>
+      <c r="R28" s="53"/>
+      <c r="S28" s="53"/>
+      <c r="T28" s="53"/>
+      <c r="U28" s="53"/>
+      <c r="V28" s="45"/>
     </row>
     <row r="29" spans="1:22" ht="27" customHeight="1">
-      <c r="A29" s="72"/>
-      <c r="B29" s="73"/>
-      <c r="C29" s="73"/>
-      <c r="D29" s="73"/>
-      <c r="E29" s="73"/>
-      <c r="F29" s="73"/>
-      <c r="G29" s="73"/>
-      <c r="H29" s="73"/>
-      <c r="I29" s="72"/>
-      <c r="J29" s="73"/>
-      <c r="K29" s="72"/>
-      <c r="L29" s="72"/>
-      <c r="M29" s="72"/>
-      <c r="N29" s="72"/>
-      <c r="O29" s="73"/>
-      <c r="P29" s="74"/>
-      <c r="Q29" s="73"/>
-      <c r="R29" s="73"/>
-      <c r="S29" s="73"/>
-      <c r="T29" s="73"/>
-      <c r="U29" s="73"/>
-      <c r="V29" s="65"/>
+      <c r="A29" s="52"/>
+      <c r="B29" s="53"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="53"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="52"/>
+      <c r="J29" s="53"/>
+      <c r="K29" s="52"/>
+      <c r="L29" s="52"/>
+      <c r="M29" s="52"/>
+      <c r="N29" s="52"/>
+      <c r="O29" s="53"/>
+      <c r="P29" s="54"/>
+      <c r="Q29" s="53"/>
+      <c r="R29" s="53"/>
+      <c r="S29" s="53"/>
+      <c r="T29" s="53"/>
+      <c r="U29" s="53"/>
+      <c r="V29" s="45"/>
     </row>
     <row r="30" spans="1:22" ht="27" customHeight="1">
-      <c r="A30" s="72"/>
-      <c r="B30" s="73"/>
-      <c r="C30" s="73"/>
-      <c r="D30" s="73"/>
-      <c r="E30" s="73"/>
-      <c r="F30" s="73"/>
-      <c r="G30" s="73"/>
-      <c r="H30" s="73"/>
-      <c r="I30" s="72"/>
-      <c r="J30" s="73"/>
-      <c r="K30" s="72"/>
-      <c r="L30" s="72"/>
-      <c r="M30" s="72"/>
-      <c r="N30" s="72"/>
-      <c r="O30" s="73"/>
-      <c r="P30" s="74"/>
-      <c r="Q30" s="73"/>
-      <c r="R30" s="73"/>
-      <c r="S30" s="73"/>
-      <c r="T30" s="73"/>
-      <c r="U30" s="73"/>
-      <c r="V30" s="65"/>
+      <c r="A30" s="52"/>
+      <c r="B30" s="53"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="53"/>
+      <c r="G30" s="53"/>
+      <c r="H30" s="53"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="53"/>
+      <c r="K30" s="52"/>
+      <c r="L30" s="52"/>
+      <c r="M30" s="52"/>
+      <c r="N30" s="52"/>
+      <c r="O30" s="53"/>
+      <c r="P30" s="54"/>
+      <c r="Q30" s="53"/>
+      <c r="R30" s="53"/>
+      <c r="S30" s="53"/>
+      <c r="T30" s="53"/>
+      <c r="U30" s="53"/>
+      <c r="V30" s="45"/>
     </row>
     <row r="31" spans="1:22" ht="27" customHeight="1">
-      <c r="A31" s="72"/>
-      <c r="B31" s="73"/>
-      <c r="C31" s="73"/>
-      <c r="D31" s="73"/>
-      <c r="E31" s="73"/>
-      <c r="F31" s="73"/>
-      <c r="G31" s="73"/>
-      <c r="H31" s="73"/>
-      <c r="I31" s="72"/>
-      <c r="J31" s="73"/>
-      <c r="K31" s="72"/>
-      <c r="L31" s="72"/>
-      <c r="M31" s="72"/>
-      <c r="N31" s="72"/>
-      <c r="O31" s="73"/>
-      <c r="P31" s="74"/>
-      <c r="Q31" s="73"/>
-      <c r="R31" s="73"/>
-      <c r="S31" s="73"/>
-      <c r="T31" s="73"/>
-      <c r="U31" s="73"/>
-      <c r="V31" s="65"/>
+      <c r="A31" s="52"/>
+      <c r="B31" s="53"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="53"/>
+      <c r="F31" s="53"/>
+      <c r="G31" s="53"/>
+      <c r="H31" s="53"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="53"/>
+      <c r="K31" s="52"/>
+      <c r="L31" s="52"/>
+      <c r="M31" s="52"/>
+      <c r="N31" s="52"/>
+      <c r="O31" s="53"/>
+      <c r="P31" s="54"/>
+      <c r="Q31" s="53"/>
+      <c r="R31" s="53"/>
+      <c r="S31" s="53"/>
+      <c r="T31" s="53"/>
+      <c r="U31" s="53"/>
+      <c r="V31" s="45"/>
     </row>
     <row r="32" spans="1:22" ht="27" customHeight="1">
-      <c r="A32" s="72"/>
-      <c r="B32" s="73"/>
-      <c r="C32" s="73"/>
-      <c r="D32" s="73"/>
-      <c r="E32" s="73"/>
-      <c r="F32" s="73"/>
-      <c r="G32" s="73"/>
-      <c r="H32" s="73"/>
-      <c r="I32" s="72"/>
-      <c r="J32" s="73"/>
-      <c r="K32" s="72"/>
-      <c r="L32" s="72"/>
-      <c r="M32" s="72"/>
-      <c r="N32" s="72"/>
-      <c r="O32" s="73"/>
-      <c r="P32" s="74"/>
-      <c r="Q32" s="73"/>
-      <c r="R32" s="73"/>
-      <c r="S32" s="73"/>
-      <c r="T32" s="73"/>
-      <c r="U32" s="73"/>
-      <c r="V32" s="65"/>
+      <c r="A32" s="52"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="53"/>
+      <c r="F32" s="53"/>
+      <c r="G32" s="53"/>
+      <c r="H32" s="53"/>
+      <c r="I32" s="52"/>
+      <c r="J32" s="53"/>
+      <c r="K32" s="52"/>
+      <c r="L32" s="52"/>
+      <c r="M32" s="52"/>
+      <c r="N32" s="52"/>
+      <c r="O32" s="53"/>
+      <c r="P32" s="54"/>
+      <c r="Q32" s="53"/>
+      <c r="R32" s="53"/>
+      <c r="S32" s="53"/>
+      <c r="T32" s="53"/>
+      <c r="U32" s="53"/>
+      <c r="V32" s="45"/>
     </row>
     <row r="33" spans="1:22" ht="27" customHeight="1">
-      <c r="A33" s="72"/>
-      <c r="B33" s="73"/>
-      <c r="C33" s="73"/>
-      <c r="D33" s="73"/>
-      <c r="E33" s="73"/>
-      <c r="F33" s="73"/>
-      <c r="G33" s="73"/>
-      <c r="H33" s="73"/>
-      <c r="I33" s="72"/>
-      <c r="J33" s="73"/>
-      <c r="K33" s="72"/>
-      <c r="L33" s="72"/>
-      <c r="M33" s="72"/>
-      <c r="N33" s="72"/>
-      <c r="O33" s="73"/>
-      <c r="P33" s="74"/>
-      <c r="Q33" s="73"/>
-      <c r="R33" s="73"/>
-      <c r="S33" s="73"/>
-      <c r="T33" s="73"/>
-      <c r="U33" s="73"/>
-      <c r="V33" s="65"/>
+      <c r="A33" s="52"/>
+      <c r="B33" s="53"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="53"/>
+      <c r="F33" s="53"/>
+      <c r="G33" s="53"/>
+      <c r="H33" s="53"/>
+      <c r="I33" s="52"/>
+      <c r="J33" s="53"/>
+      <c r="K33" s="52"/>
+      <c r="L33" s="52"/>
+      <c r="M33" s="52"/>
+      <c r="N33" s="52"/>
+      <c r="O33" s="53"/>
+      <c r="P33" s="54"/>
+      <c r="Q33" s="53"/>
+      <c r="R33" s="53"/>
+      <c r="S33" s="53"/>
+      <c r="T33" s="53"/>
+      <c r="U33" s="53"/>
+      <c r="V33" s="45"/>
     </row>
     <row r="34" spans="1:22" ht="27" customHeight="1">
-      <c r="A34" s="72"/>
-      <c r="B34" s="73"/>
-      <c r="C34" s="73"/>
-      <c r="D34" s="73"/>
-      <c r="E34" s="73"/>
-      <c r="F34" s="73"/>
-      <c r="G34" s="73"/>
-      <c r="H34" s="73"/>
-      <c r="I34" s="72"/>
-      <c r="J34" s="73"/>
-      <c r="K34" s="72"/>
-      <c r="L34" s="72"/>
-      <c r="M34" s="72"/>
-      <c r="N34" s="72"/>
-      <c r="O34" s="73"/>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="73"/>
-      <c r="R34" s="73"/>
-      <c r="S34" s="73"/>
-      <c r="T34" s="73"/>
-      <c r="U34" s="73"/>
-      <c r="V34" s="65"/>
+      <c r="A34" s="52"/>
+      <c r="B34" s="53"/>
+      <c r="C34" s="53"/>
+      <c r="D34" s="53"/>
+      <c r="E34" s="53"/>
+      <c r="F34" s="53"/>
+      <c r="G34" s="53"/>
+      <c r="H34" s="53"/>
+      <c r="I34" s="52"/>
+      <c r="J34" s="53"/>
+      <c r="K34" s="52"/>
+      <c r="L34" s="52"/>
+      <c r="M34" s="52"/>
+      <c r="N34" s="52"/>
+      <c r="O34" s="53"/>
+      <c r="P34" s="54"/>
+      <c r="Q34" s="53"/>
+      <c r="R34" s="53"/>
+      <c r="S34" s="53"/>
+      <c r="T34" s="53"/>
+      <c r="U34" s="53"/>
+      <c r="V34" s="45"/>
     </row>
     <row r="35" spans="1:22" ht="27" customHeight="1">
-      <c r="A35" s="72"/>
-      <c r="B35" s="73"/>
-      <c r="C35" s="73"/>
-      <c r="D35" s="73"/>
-      <c r="E35" s="73"/>
-      <c r="F35" s="73"/>
-      <c r="G35" s="73"/>
-      <c r="H35" s="73"/>
-      <c r="I35" s="72"/>
-      <c r="J35" s="73"/>
-      <c r="K35" s="72"/>
-      <c r="L35" s="72"/>
-      <c r="M35" s="72"/>
-      <c r="N35" s="72"/>
-      <c r="O35" s="73"/>
-      <c r="P35" s="74"/>
-      <c r="Q35" s="73"/>
-      <c r="R35" s="73"/>
-      <c r="S35" s="73"/>
-      <c r="T35" s="73"/>
-      <c r="U35" s="73"/>
-      <c r="V35" s="65"/>
+      <c r="A35" s="52"/>
+      <c r="B35" s="53"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="53"/>
+      <c r="E35" s="53"/>
+      <c r="F35" s="53"/>
+      <c r="G35" s="53"/>
+      <c r="H35" s="53"/>
+      <c r="I35" s="52"/>
+      <c r="J35" s="53"/>
+      <c r="K35" s="52"/>
+      <c r="L35" s="52"/>
+      <c r="M35" s="52"/>
+      <c r="N35" s="52"/>
+      <c r="O35" s="53"/>
+      <c r="P35" s="54"/>
+      <c r="Q35" s="53"/>
+      <c r="R35" s="53"/>
+      <c r="S35" s="53"/>
+      <c r="T35" s="53"/>
+      <c r="U35" s="53"/>
+      <c r="V35" s="45"/>
     </row>
     <row r="36" spans="1:22" ht="27" customHeight="1">
-      <c r="A36" s="72"/>
-      <c r="B36" s="73"/>
-      <c r="C36" s="73"/>
-      <c r="D36" s="73"/>
-      <c r="E36" s="73"/>
-      <c r="F36" s="73"/>
-      <c r="G36" s="73"/>
-      <c r="H36" s="73"/>
-      <c r="I36" s="72"/>
-      <c r="J36" s="73"/>
-      <c r="K36" s="72"/>
-      <c r="L36" s="72"/>
-      <c r="M36" s="72"/>
-      <c r="N36" s="72"/>
-      <c r="O36" s="73"/>
-      <c r="P36" s="74"/>
-      <c r="Q36" s="73"/>
-      <c r="R36" s="73"/>
-      <c r="S36" s="73"/>
-      <c r="T36" s="73"/>
-      <c r="U36" s="73"/>
-      <c r="V36" s="65"/>
+      <c r="A36" s="52"/>
+      <c r="B36" s="53"/>
+      <c r="C36" s="53"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="53"/>
+      <c r="G36" s="53"/>
+      <c r="H36" s="53"/>
+      <c r="I36" s="52"/>
+      <c r="J36" s="53"/>
+      <c r="K36" s="52"/>
+      <c r="L36" s="52"/>
+      <c r="M36" s="52"/>
+      <c r="N36" s="52"/>
+      <c r="O36" s="53"/>
+      <c r="P36" s="54"/>
+      <c r="Q36" s="53"/>
+      <c r="R36" s="53"/>
+      <c r="S36" s="53"/>
+      <c r="T36" s="53"/>
+      <c r="U36" s="53"/>
+      <c r="V36" s="45"/>
     </row>
     <row r="37" spans="1:22" ht="27" customHeight="1">
-      <c r="A37" s="72"/>
-      <c r="B37" s="73"/>
-      <c r="C37" s="73"/>
-      <c r="D37" s="73"/>
-      <c r="E37" s="73"/>
-      <c r="F37" s="73"/>
-      <c r="G37" s="73"/>
-      <c r="H37" s="73"/>
-      <c r="I37" s="72"/>
-      <c r="J37" s="73"/>
-      <c r="K37" s="72"/>
-      <c r="L37" s="72"/>
-      <c r="M37" s="72"/>
-      <c r="N37" s="72"/>
-      <c r="O37" s="73"/>
-      <c r="P37" s="74"/>
-      <c r="Q37" s="73"/>
-      <c r="R37" s="73"/>
-      <c r="S37" s="73"/>
-      <c r="T37" s="73"/>
-      <c r="U37" s="73"/>
-      <c r="V37" s="65"/>
+      <c r="A37" s="52"/>
+      <c r="B37" s="53"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="53"/>
+      <c r="G37" s="53"/>
+      <c r="H37" s="53"/>
+      <c r="I37" s="52"/>
+      <c r="J37" s="53"/>
+      <c r="K37" s="52"/>
+      <c r="L37" s="52"/>
+      <c r="M37" s="52"/>
+      <c r="N37" s="52"/>
+      <c r="O37" s="53"/>
+      <c r="P37" s="54"/>
+      <c r="Q37" s="53"/>
+      <c r="R37" s="53"/>
+      <c r="S37" s="53"/>
+      <c r="T37" s="53"/>
+      <c r="U37" s="53"/>
+      <c r="V37" s="45"/>
     </row>
     <row r="38" spans="1:22" ht="27" customHeight="1">
-      <c r="A38" s="72"/>
-      <c r="B38" s="73"/>
-      <c r="C38" s="73"/>
-      <c r="D38" s="73"/>
-      <c r="E38" s="73"/>
-      <c r="F38" s="73"/>
-      <c r="G38" s="73"/>
-      <c r="H38" s="73"/>
-      <c r="I38" s="72"/>
-      <c r="J38" s="73"/>
-      <c r="K38" s="72"/>
-      <c r="L38" s="72"/>
-      <c r="M38" s="72"/>
-      <c r="N38" s="72"/>
-      <c r="O38" s="73"/>
-      <c r="P38" s="74"/>
-      <c r="Q38" s="73"/>
-      <c r="R38" s="73"/>
-      <c r="S38" s="73"/>
-      <c r="T38" s="73"/>
-      <c r="U38" s="73"/>
-      <c r="V38" s="65"/>
+      <c r="A38" s="52"/>
+      <c r="B38" s="53"/>
+      <c r="C38" s="53"/>
+      <c r="D38" s="53"/>
+      <c r="E38" s="53"/>
+      <c r="F38" s="53"/>
+      <c r="G38" s="53"/>
+      <c r="H38" s="53"/>
+      <c r="I38" s="52"/>
+      <c r="J38" s="53"/>
+      <c r="K38" s="52"/>
+      <c r="L38" s="52"/>
+      <c r="M38" s="52"/>
+      <c r="N38" s="52"/>
+      <c r="O38" s="53"/>
+      <c r="P38" s="54"/>
+      <c r="Q38" s="53"/>
+      <c r="R38" s="53"/>
+      <c r="S38" s="53"/>
+      <c r="T38" s="53"/>
+      <c r="U38" s="53"/>
+      <c r="V38" s="45"/>
     </row>
     <row r="39" spans="1:22" ht="27" customHeight="1">
-      <c r="A39" s="72"/>
-      <c r="B39" s="73"/>
-      <c r="C39" s="73"/>
-      <c r="D39" s="73"/>
-      <c r="E39" s="73"/>
-      <c r="F39" s="73"/>
-      <c r="G39" s="73"/>
-      <c r="H39" s="73"/>
-      <c r="I39" s="72"/>
-      <c r="J39" s="73"/>
-      <c r="K39" s="72"/>
-      <c r="L39" s="72"/>
-      <c r="M39" s="72"/>
-      <c r="N39" s="72"/>
-      <c r="O39" s="73"/>
-      <c r="P39" s="74"/>
-      <c r="Q39" s="73"/>
-      <c r="R39" s="73"/>
-      <c r="S39" s="73"/>
-      <c r="T39" s="73"/>
-      <c r="U39" s="73"/>
-      <c r="V39" s="65"/>
+      <c r="A39" s="52"/>
+      <c r="B39" s="53"/>
+      <c r="C39" s="53"/>
+      <c r="D39" s="53"/>
+      <c r="E39" s="53"/>
+      <c r="F39" s="53"/>
+      <c r="G39" s="53"/>
+      <c r="H39" s="53"/>
+      <c r="I39" s="52"/>
+      <c r="J39" s="53"/>
+      <c r="K39" s="52"/>
+      <c r="L39" s="52"/>
+      <c r="M39" s="52"/>
+      <c r="N39" s="52"/>
+      <c r="O39" s="53"/>
+      <c r="P39" s="54"/>
+      <c r="Q39" s="53"/>
+      <c r="R39" s="53"/>
+      <c r="S39" s="53"/>
+      <c r="T39" s="53"/>
+      <c r="U39" s="53"/>
+      <c r="V39" s="45"/>
     </row>
     <row r="40" spans="1:22" ht="27" customHeight="1">
-      <c r="A40" s="72"/>
-      <c r="B40" s="73"/>
-      <c r="C40" s="73"/>
-      <c r="D40" s="73"/>
-      <c r="E40" s="73"/>
-      <c r="F40" s="73"/>
-      <c r="G40" s="73"/>
-      <c r="H40" s="73"/>
-      <c r="I40" s="72"/>
-      <c r="J40" s="73"/>
-      <c r="K40" s="72"/>
-      <c r="L40" s="72"/>
-      <c r="M40" s="72"/>
-      <c r="N40" s="72"/>
-      <c r="O40" s="73"/>
-      <c r="P40" s="74"/>
-      <c r="Q40" s="73"/>
-      <c r="R40" s="73"/>
-      <c r="S40" s="73"/>
-      <c r="T40" s="73"/>
-      <c r="U40" s="73"/>
-      <c r="V40" s="65"/>
+      <c r="A40" s="52"/>
+      <c r="B40" s="53"/>
+      <c r="C40" s="53"/>
+      <c r="D40" s="53"/>
+      <c r="E40" s="53"/>
+      <c r="F40" s="53"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="53"/>
+      <c r="I40" s="52"/>
+      <c r="J40" s="53"/>
+      <c r="K40" s="52"/>
+      <c r="L40" s="52"/>
+      <c r="M40" s="52"/>
+      <c r="N40" s="52"/>
+      <c r="O40" s="53"/>
+      <c r="P40" s="54"/>
+      <c r="Q40" s="53"/>
+      <c r="R40" s="53"/>
+      <c r="S40" s="53"/>
+      <c r="T40" s="53"/>
+      <c r="U40" s="53"/>
+      <c r="V40" s="45"/>
     </row>
     <row r="41" spans="1:22" ht="27" customHeight="1">
-      <c r="A41" s="72"/>
-      <c r="B41" s="73"/>
-      <c r="C41" s="73"/>
-      <c r="D41" s="73"/>
-      <c r="E41" s="73"/>
-      <c r="F41" s="73"/>
-      <c r="G41" s="73"/>
-      <c r="H41" s="73"/>
-      <c r="I41" s="72"/>
-      <c r="J41" s="73"/>
-      <c r="K41" s="72"/>
-      <c r="L41" s="72"/>
-      <c r="M41" s="72"/>
-      <c r="N41" s="72"/>
-      <c r="O41" s="73"/>
-      <c r="P41" s="74"/>
-      <c r="Q41" s="73"/>
-      <c r="R41" s="73"/>
-      <c r="S41" s="73"/>
-      <c r="T41" s="73"/>
-      <c r="U41" s="73"/>
-      <c r="V41" s="65"/>
+      <c r="A41" s="52"/>
+      <c r="B41" s="53"/>
+      <c r="C41" s="53"/>
+      <c r="D41" s="53"/>
+      <c r="E41" s="53"/>
+      <c r="F41" s="53"/>
+      <c r="G41" s="53"/>
+      <c r="H41" s="53"/>
+      <c r="I41" s="52"/>
+      <c r="J41" s="53"/>
+      <c r="K41" s="52"/>
+      <c r="L41" s="52"/>
+      <c r="M41" s="52"/>
+      <c r="N41" s="52"/>
+      <c r="O41" s="53"/>
+      <c r="P41" s="54"/>
+      <c r="Q41" s="53"/>
+      <c r="R41" s="53"/>
+      <c r="S41" s="53"/>
+      <c r="T41" s="53"/>
+      <c r="U41" s="53"/>
+      <c r="V41" s="45"/>
     </row>
     <row r="42" spans="1:22" ht="27" customHeight="1">
-      <c r="A42" s="72"/>
-      <c r="B42" s="73"/>
-      <c r="C42" s="73"/>
-      <c r="D42" s="73"/>
-      <c r="E42" s="73"/>
-      <c r="F42" s="73"/>
-      <c r="G42" s="73"/>
-      <c r="H42" s="73"/>
-      <c r="I42" s="72"/>
-      <c r="J42" s="73"/>
-      <c r="K42" s="72"/>
-      <c r="L42" s="72"/>
-      <c r="M42" s="72"/>
-      <c r="N42" s="72"/>
-      <c r="O42" s="73"/>
-      <c r="P42" s="74"/>
-      <c r="Q42" s="73"/>
-      <c r="R42" s="73"/>
-      <c r="S42" s="73"/>
-      <c r="T42" s="73"/>
-      <c r="U42" s="73"/>
-      <c r="V42" s="65"/>
+      <c r="A42" s="52"/>
+      <c r="B42" s="53"/>
+      <c r="C42" s="53"/>
+      <c r="D42" s="53"/>
+      <c r="E42" s="53"/>
+      <c r="F42" s="53"/>
+      <c r="G42" s="53"/>
+      <c r="H42" s="53"/>
+      <c r="I42" s="52"/>
+      <c r="J42" s="53"/>
+      <c r="K42" s="52"/>
+      <c r="L42" s="52"/>
+      <c r="M42" s="52"/>
+      <c r="N42" s="52"/>
+      <c r="O42" s="53"/>
+      <c r="P42" s="54"/>
+      <c r="Q42" s="53"/>
+      <c r="R42" s="53"/>
+      <c r="S42" s="53"/>
+      <c r="T42" s="53"/>
+      <c r="U42" s="53"/>
+      <c r="V42" s="45"/>
     </row>
     <row r="43" spans="1:22" ht="27" customHeight="1">
-      <c r="A43" s="72"/>
-      <c r="B43" s="73"/>
-      <c r="C43" s="73"/>
-      <c r="D43" s="73"/>
-      <c r="E43" s="73"/>
-      <c r="F43" s="73"/>
-      <c r="G43" s="73"/>
-      <c r="H43" s="73"/>
-      <c r="I43" s="72"/>
-      <c r="J43" s="73"/>
-      <c r="K43" s="72"/>
-      <c r="L43" s="72"/>
-      <c r="M43" s="72"/>
-      <c r="N43" s="72"/>
-      <c r="O43" s="73"/>
-      <c r="P43" s="74"/>
-      <c r="Q43" s="73"/>
-      <c r="R43" s="73"/>
-      <c r="S43" s="73"/>
-      <c r="T43" s="73"/>
-      <c r="U43" s="73"/>
-      <c r="V43" s="65"/>
+      <c r="A43" s="52"/>
+      <c r="B43" s="53"/>
+      <c r="C43" s="53"/>
+      <c r="D43" s="53"/>
+      <c r="E43" s="53"/>
+      <c r="F43" s="53"/>
+      <c r="G43" s="53"/>
+      <c r="H43" s="53"/>
+      <c r="I43" s="52"/>
+      <c r="J43" s="53"/>
+      <c r="K43" s="52"/>
+      <c r="L43" s="52"/>
+      <c r="M43" s="52"/>
+      <c r="N43" s="52"/>
+      <c r="O43" s="53"/>
+      <c r="P43" s="54"/>
+      <c r="Q43" s="53"/>
+      <c r="R43" s="53"/>
+      <c r="S43" s="53"/>
+      <c r="T43" s="53"/>
+      <c r="U43" s="53"/>
+      <c r="V43" s="45"/>
     </row>
     <row r="44" spans="1:22" ht="27" customHeight="1">
-      <c r="A44" s="72"/>
-      <c r="B44" s="73"/>
-      <c r="C44" s="73"/>
-      <c r="D44" s="73"/>
-      <c r="E44" s="73"/>
-      <c r="F44" s="73"/>
-      <c r="G44" s="73"/>
-      <c r="H44" s="73"/>
-      <c r="I44" s="72"/>
-      <c r="J44" s="73"/>
-      <c r="K44" s="72"/>
-      <c r="L44" s="72"/>
-      <c r="M44" s="72"/>
-      <c r="N44" s="72"/>
-      <c r="O44" s="73"/>
-      <c r="P44" s="74"/>
-      <c r="Q44" s="73"/>
-      <c r="R44" s="73"/>
-      <c r="S44" s="73"/>
-      <c r="T44" s="73"/>
-      <c r="U44" s="73"/>
-      <c r="V44" s="65"/>
+      <c r="A44" s="52"/>
+      <c r="B44" s="53"/>
+      <c r="C44" s="53"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="53"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="52"/>
+      <c r="J44" s="53"/>
+      <c r="K44" s="52"/>
+      <c r="L44" s="52"/>
+      <c r="M44" s="52"/>
+      <c r="N44" s="52"/>
+      <c r="O44" s="53"/>
+      <c r="P44" s="54"/>
+      <c r="Q44" s="53"/>
+      <c r="R44" s="53"/>
+      <c r="S44" s="53"/>
+      <c r="T44" s="53"/>
+      <c r="U44" s="53"/>
+      <c r="V44" s="45"/>
     </row>
     <row r="45" spans="1:22" ht="27" customHeight="1">
-      <c r="A45" s="72"/>
-      <c r="B45" s="73"/>
-      <c r="C45" s="73"/>
-      <c r="D45" s="73"/>
-      <c r="E45" s="73"/>
-      <c r="F45" s="73"/>
-      <c r="G45" s="73"/>
-      <c r="H45" s="73"/>
-      <c r="I45" s="72"/>
-      <c r="J45" s="73"/>
-      <c r="K45" s="72"/>
-      <c r="L45" s="72"/>
-      <c r="M45" s="72"/>
-      <c r="N45" s="72"/>
-      <c r="O45" s="73"/>
-      <c r="P45" s="74"/>
-      <c r="Q45" s="73"/>
-      <c r="R45" s="73"/>
-      <c r="S45" s="73"/>
-      <c r="T45" s="73"/>
-      <c r="U45" s="73"/>
-      <c r="V45" s="65"/>
+      <c r="A45" s="52"/>
+      <c r="B45" s="53"/>
+      <c r="C45" s="53"/>
+      <c r="D45" s="53"/>
+      <c r="E45" s="53"/>
+      <c r="F45" s="53"/>
+      <c r="G45" s="53"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="52"/>
+      <c r="J45" s="53"/>
+      <c r="K45" s="52"/>
+      <c r="L45" s="52"/>
+      <c r="M45" s="52"/>
+      <c r="N45" s="52"/>
+      <c r="O45" s="53"/>
+      <c r="P45" s="54"/>
+      <c r="Q45" s="53"/>
+      <c r="R45" s="53"/>
+      <c r="S45" s="53"/>
+      <c r="T45" s="53"/>
+      <c r="U45" s="53"/>
+      <c r="V45" s="45"/>
     </row>
     <row r="46" spans="1:22" ht="27" customHeight="1">
-      <c r="A46" s="72"/>
-      <c r="B46" s="73"/>
-      <c r="C46" s="73"/>
-      <c r="D46" s="73"/>
-      <c r="E46" s="73"/>
-      <c r="F46" s="73"/>
-      <c r="G46" s="73"/>
-      <c r="H46" s="73"/>
-      <c r="I46" s="72"/>
-      <c r="J46" s="73"/>
-      <c r="K46" s="72"/>
-      <c r="L46" s="72"/>
-      <c r="M46" s="72"/>
-      <c r="N46" s="72"/>
-      <c r="O46" s="73"/>
-      <c r="P46" s="74"/>
-      <c r="Q46" s="73"/>
-      <c r="R46" s="73"/>
-      <c r="S46" s="73"/>
-      <c r="T46" s="73"/>
-      <c r="U46" s="73"/>
-      <c r="V46" s="65"/>
+      <c r="A46" s="52"/>
+      <c r="B46" s="53"/>
+      <c r="C46" s="53"/>
+      <c r="D46" s="53"/>
+      <c r="E46" s="53"/>
+      <c r="F46" s="53"/>
+      <c r="G46" s="53"/>
+      <c r="H46" s="53"/>
+      <c r="I46" s="52"/>
+      <c r="J46" s="53"/>
+      <c r="K46" s="52"/>
+      <c r="L46" s="52"/>
+      <c r="M46" s="52"/>
+      <c r="N46" s="52"/>
+      <c r="O46" s="53"/>
+      <c r="P46" s="54"/>
+      <c r="Q46" s="53"/>
+      <c r="R46" s="53"/>
+      <c r="S46" s="53"/>
+      <c r="T46" s="53"/>
+      <c r="U46" s="53"/>
+      <c r="V46" s="45"/>
     </row>
     <row r="47" spans="1:22" ht="27" customHeight="1">
-      <c r="A47" s="72"/>
-      <c r="B47" s="73"/>
-      <c r="C47" s="73"/>
-      <c r="D47" s="73"/>
-      <c r="E47" s="73"/>
-      <c r="F47" s="73"/>
-      <c r="G47" s="73"/>
-      <c r="H47" s="73"/>
-      <c r="I47" s="72"/>
-      <c r="J47" s="73"/>
-      <c r="K47" s="72"/>
-      <c r="L47" s="72"/>
-      <c r="M47" s="72"/>
-      <c r="N47" s="72"/>
-      <c r="O47" s="73"/>
-      <c r="P47" s="74"/>
-      <c r="Q47" s="73"/>
-      <c r="R47" s="73"/>
-      <c r="S47" s="73"/>
-      <c r="T47" s="73"/>
-      <c r="U47" s="73"/>
-      <c r="V47" s="65"/>
+      <c r="A47" s="52"/>
+      <c r="B47" s="53"/>
+      <c r="C47" s="53"/>
+      <c r="D47" s="53"/>
+      <c r="E47" s="53"/>
+      <c r="F47" s="53"/>
+      <c r="G47" s="53"/>
+      <c r="H47" s="53"/>
+      <c r="I47" s="52"/>
+      <c r="J47" s="53"/>
+      <c r="K47" s="52"/>
+      <c r="L47" s="52"/>
+      <c r="M47" s="52"/>
+      <c r="N47" s="52"/>
+      <c r="O47" s="53"/>
+      <c r="P47" s="54"/>
+      <c r="Q47" s="53"/>
+      <c r="R47" s="53"/>
+      <c r="S47" s="53"/>
+      <c r="T47" s="53"/>
+      <c r="U47" s="53"/>
+      <c r="V47" s="45"/>
     </row>
     <row r="48" spans="1:22" ht="27" customHeight="1">
-      <c r="A48" s="72"/>
-      <c r="B48" s="73"/>
-      <c r="C48" s="73"/>
-      <c r="D48" s="73"/>
-      <c r="E48" s="73"/>
-      <c r="F48" s="73"/>
-      <c r="G48" s="73"/>
-      <c r="H48" s="73"/>
-      <c r="I48" s="72"/>
-      <c r="J48" s="73"/>
-      <c r="K48" s="72"/>
-      <c r="L48" s="72"/>
-      <c r="M48" s="72"/>
-      <c r="N48" s="72"/>
-      <c r="O48" s="73"/>
-      <c r="P48" s="74"/>
-      <c r="Q48" s="73"/>
-      <c r="R48" s="73"/>
-      <c r="S48" s="73"/>
-      <c r="T48" s="73"/>
-      <c r="U48" s="73"/>
-      <c r="V48" s="65"/>
+      <c r="A48" s="52"/>
+      <c r="B48" s="53"/>
+      <c r="C48" s="53"/>
+      <c r="D48" s="53"/>
+      <c r="E48" s="53"/>
+      <c r="F48" s="53"/>
+      <c r="G48" s="53"/>
+      <c r="H48" s="53"/>
+      <c r="I48" s="52"/>
+      <c r="J48" s="53"/>
+      <c r="K48" s="52"/>
+      <c r="L48" s="52"/>
+      <c r="M48" s="52"/>
+      <c r="N48" s="52"/>
+      <c r="O48" s="53"/>
+      <c r="P48" s="54"/>
+      <c r="Q48" s="53"/>
+      <c r="R48" s="53"/>
+      <c r="S48" s="53"/>
+      <c r="T48" s="53"/>
+      <c r="U48" s="53"/>
+      <c r="V48" s="45"/>
     </row>
     <row r="49" spans="1:22" ht="27" customHeight="1">
-      <c r="A49" s="72"/>
-      <c r="B49" s="73"/>
-      <c r="C49" s="73"/>
-      <c r="D49" s="73"/>
-      <c r="E49" s="73"/>
-      <c r="F49" s="73"/>
-      <c r="G49" s="73"/>
-      <c r="H49" s="73"/>
-      <c r="I49" s="72"/>
-      <c r="J49" s="73"/>
-      <c r="K49" s="72"/>
-      <c r="L49" s="72"/>
-      <c r="M49" s="72"/>
-      <c r="N49" s="72"/>
-      <c r="O49" s="73"/>
-      <c r="P49" s="74"/>
-      <c r="Q49" s="73"/>
-      <c r="R49" s="73"/>
-      <c r="S49" s="73"/>
-      <c r="T49" s="73"/>
-      <c r="U49" s="73"/>
-      <c r="V49" s="65"/>
+      <c r="A49" s="52"/>
+      <c r="B49" s="53"/>
+      <c r="C49" s="53"/>
+      <c r="D49" s="53"/>
+      <c r="E49" s="53"/>
+      <c r="F49" s="53"/>
+      <c r="G49" s="53"/>
+      <c r="H49" s="53"/>
+      <c r="I49" s="52"/>
+      <c r="J49" s="53"/>
+      <c r="K49" s="52"/>
+      <c r="L49" s="52"/>
+      <c r="M49" s="52"/>
+      <c r="N49" s="52"/>
+      <c r="O49" s="53"/>
+      <c r="P49" s="54"/>
+      <c r="Q49" s="53"/>
+      <c r="R49" s="53"/>
+      <c r="S49" s="53"/>
+      <c r="T49" s="53"/>
+      <c r="U49" s="53"/>
+      <c r="V49" s="45"/>
     </row>
     <row r="50" spans="1:22" ht="27" customHeight="1">
-      <c r="A50" s="72"/>
-      <c r="B50" s="73"/>
-      <c r="C50" s="73"/>
-      <c r="D50" s="73"/>
-      <c r="E50" s="73"/>
-      <c r="F50" s="73"/>
-      <c r="G50" s="73"/>
-      <c r="H50" s="73"/>
-      <c r="I50" s="72"/>
-      <c r="J50" s="73"/>
-      <c r="K50" s="72"/>
-      <c r="L50" s="72"/>
-      <c r="M50" s="72"/>
-      <c r="N50" s="72"/>
-      <c r="O50" s="73"/>
-      <c r="P50" s="74"/>
-      <c r="Q50" s="73"/>
-      <c r="R50" s="73"/>
-      <c r="S50" s="73"/>
-      <c r="T50" s="73"/>
-      <c r="U50" s="73"/>
-      <c r="V50" s="65"/>
+      <c r="A50" s="52"/>
+      <c r="B50" s="53"/>
+      <c r="C50" s="53"/>
+      <c r="D50" s="53"/>
+      <c r="E50" s="53"/>
+      <c r="F50" s="53"/>
+      <c r="G50" s="53"/>
+      <c r="H50" s="53"/>
+      <c r="I50" s="52"/>
+      <c r="J50" s="53"/>
+      <c r="K50" s="52"/>
+      <c r="L50" s="52"/>
+      <c r="M50" s="52"/>
+      <c r="N50" s="52"/>
+      <c r="O50" s="53"/>
+      <c r="P50" s="54"/>
+      <c r="Q50" s="53"/>
+      <c r="R50" s="53"/>
+      <c r="S50" s="53"/>
+      <c r="T50" s="53"/>
+      <c r="U50" s="53"/>
+      <c r="V50" s="45"/>
     </row>
     <row r="51" spans="1:22" ht="27" customHeight="1">
-      <c r="A51" s="72"/>
-      <c r="B51" s="73"/>
-      <c r="C51" s="73"/>
-      <c r="D51" s="73"/>
-      <c r="E51" s="73"/>
-      <c r="F51" s="73"/>
-      <c r="G51" s="73"/>
-      <c r="H51" s="73"/>
-      <c r="I51" s="72"/>
-      <c r="J51" s="73"/>
-      <c r="K51" s="72"/>
-      <c r="L51" s="72"/>
-      <c r="M51" s="72"/>
-      <c r="N51" s="72"/>
-      <c r="O51" s="73"/>
-      <c r="P51" s="74"/>
-      <c r="Q51" s="73"/>
-      <c r="R51" s="73"/>
-      <c r="S51" s="73"/>
-      <c r="T51" s="73"/>
-      <c r="U51" s="73"/>
-      <c r="V51" s="65"/>
+      <c r="A51" s="52"/>
+      <c r="B51" s="53"/>
+      <c r="C51" s="53"/>
+      <c r="D51" s="53"/>
+      <c r="E51" s="53"/>
+      <c r="F51" s="53"/>
+      <c r="G51" s="53"/>
+      <c r="H51" s="53"/>
+      <c r="I51" s="52"/>
+      <c r="J51" s="53"/>
+      <c r="K51" s="52"/>
+      <c r="L51" s="52"/>
+      <c r="M51" s="52"/>
+      <c r="N51" s="52"/>
+      <c r="O51" s="53"/>
+      <c r="P51" s="54"/>
+      <c r="Q51" s="53"/>
+      <c r="R51" s="53"/>
+      <c r="S51" s="53"/>
+      <c r="T51" s="53"/>
+      <c r="U51" s="53"/>
+      <c r="V51" s="45"/>
     </row>
     <row r="52" spans="1:22" ht="27" customHeight="1">
-      <c r="A52" s="72"/>
-      <c r="B52" s="73"/>
-      <c r="C52" s="73"/>
-      <c r="D52" s="73"/>
-      <c r="E52" s="73"/>
-      <c r="F52" s="73"/>
-      <c r="G52" s="73"/>
-      <c r="H52" s="73"/>
-      <c r="I52" s="72"/>
-      <c r="J52" s="73"/>
-      <c r="K52" s="72"/>
-      <c r="L52" s="72"/>
-      <c r="M52" s="72"/>
-      <c r="N52" s="72"/>
-      <c r="O52" s="73"/>
-      <c r="P52" s="74"/>
-      <c r="Q52" s="73"/>
-      <c r="R52" s="73"/>
-      <c r="S52" s="73"/>
-      <c r="T52" s="73"/>
-      <c r="U52" s="73"/>
-      <c r="V52" s="65"/>
+      <c r="A52" s="52"/>
+      <c r="B52" s="53"/>
+      <c r="C52" s="53"/>
+      <c r="D52" s="53"/>
+      <c r="E52" s="53"/>
+      <c r="F52" s="53"/>
+      <c r="G52" s="53"/>
+      <c r="H52" s="53"/>
+      <c r="I52" s="52"/>
+      <c r="J52" s="53"/>
+      <c r="K52" s="52"/>
+      <c r="L52" s="52"/>
+      <c r="M52" s="52"/>
+      <c r="N52" s="52"/>
+      <c r="O52" s="53"/>
+      <c r="P52" s="54"/>
+      <c r="Q52" s="53"/>
+      <c r="R52" s="53"/>
+      <c r="S52" s="53"/>
+      <c r="T52" s="53"/>
+      <c r="U52" s="53"/>
+      <c r="V52" s="45"/>
     </row>
     <row r="53" spans="1:22" ht="27" customHeight="1">
-      <c r="A53" s="72"/>
-      <c r="B53" s="73"/>
-      <c r="C53" s="73"/>
-      <c r="D53" s="73"/>
-      <c r="E53" s="73"/>
-      <c r="F53" s="73"/>
-      <c r="G53" s="73"/>
-      <c r="H53" s="73"/>
-      <c r="I53" s="72"/>
-      <c r="J53" s="73"/>
-      <c r="K53" s="72"/>
-      <c r="L53" s="72"/>
-      <c r="M53" s="72"/>
-      <c r="N53" s="72"/>
-      <c r="O53" s="73"/>
-      <c r="P53" s="74"/>
-      <c r="Q53" s="73"/>
-      <c r="R53" s="73"/>
-      <c r="S53" s="73"/>
-      <c r="T53" s="73"/>
-      <c r="U53" s="73"/>
-      <c r="V53" s="65"/>
+      <c r="A53" s="52"/>
+      <c r="B53" s="53"/>
+      <c r="C53" s="53"/>
+      <c r="D53" s="53"/>
+      <c r="E53" s="53"/>
+      <c r="F53" s="53"/>
+      <c r="G53" s="53"/>
+      <c r="H53" s="53"/>
+      <c r="I53" s="52"/>
+      <c r="J53" s="53"/>
+      <c r="K53" s="52"/>
+      <c r="L53" s="52"/>
+      <c r="M53" s="52"/>
+      <c r="N53" s="52"/>
+      <c r="O53" s="53"/>
+      <c r="P53" s="54"/>
+      <c r="Q53" s="53"/>
+      <c r="R53" s="53"/>
+      <c r="S53" s="53"/>
+      <c r="T53" s="53"/>
+      <c r="U53" s="53"/>
+      <c r="V53" s="45"/>
     </row>
     <row r="54" spans="1:22" ht="27" customHeight="1">
-      <c r="A54" s="72"/>
-      <c r="B54" s="73"/>
-      <c r="C54" s="73"/>
-      <c r="D54" s="73"/>
-      <c r="E54" s="73"/>
-      <c r="F54" s="73"/>
-      <c r="G54" s="73"/>
-      <c r="H54" s="73"/>
-      <c r="I54" s="72"/>
-      <c r="J54" s="73"/>
-      <c r="K54" s="72"/>
-      <c r="L54" s="72"/>
-      <c r="M54" s="72"/>
-      <c r="N54" s="72"/>
-      <c r="O54" s="73"/>
-      <c r="P54" s="74"/>
-      <c r="Q54" s="73"/>
-      <c r="R54" s="73"/>
-      <c r="S54" s="73"/>
-      <c r="T54" s="73"/>
-      <c r="U54" s="73"/>
-      <c r="V54" s="65"/>
+      <c r="A54" s="52"/>
+      <c r="B54" s="53"/>
+      <c r="C54" s="53"/>
+      <c r="D54" s="53"/>
+      <c r="E54" s="53"/>
+      <c r="F54" s="53"/>
+      <c r="G54" s="53"/>
+      <c r="H54" s="53"/>
+      <c r="I54" s="52"/>
+      <c r="J54" s="53"/>
+      <c r="K54" s="52"/>
+      <c r="L54" s="52"/>
+      <c r="M54" s="52"/>
+      <c r="N54" s="52"/>
+      <c r="O54" s="53"/>
+      <c r="P54" s="54"/>
+      <c r="Q54" s="53"/>
+      <c r="R54" s="53"/>
+      <c r="S54" s="53"/>
+      <c r="T54" s="53"/>
+      <c r="U54" s="53"/>
+      <c r="V54" s="45"/>
     </row>
     <row r="55" spans="1:22" ht="27" customHeight="1">
-      <c r="A55" s="72"/>
-      <c r="B55" s="73"/>
-      <c r="C55" s="73"/>
-      <c r="D55" s="73"/>
-      <c r="E55" s="73"/>
-      <c r="F55" s="73"/>
-      <c r="G55" s="73"/>
-      <c r="H55" s="73"/>
-      <c r="I55" s="72"/>
-      <c r="J55" s="73"/>
-      <c r="K55" s="72"/>
-      <c r="L55" s="72"/>
-      <c r="M55" s="72"/>
-      <c r="N55" s="72"/>
-      <c r="O55" s="73"/>
-      <c r="P55" s="74"/>
-      <c r="Q55" s="73"/>
-      <c r="R55" s="73"/>
-      <c r="S55" s="73"/>
-      <c r="T55" s="73"/>
-      <c r="U55" s="73"/>
-      <c r="V55" s="65"/>
+      <c r="A55" s="52"/>
+      <c r="B55" s="53"/>
+      <c r="C55" s="53"/>
+      <c r="D55" s="53"/>
+      <c r="E55" s="53"/>
+      <c r="F55" s="53"/>
+      <c r="G55" s="53"/>
+      <c r="H55" s="53"/>
+      <c r="I55" s="52"/>
+      <c r="J55" s="53"/>
+      <c r="K55" s="52"/>
+      <c r="L55" s="52"/>
+      <c r="M55" s="52"/>
+      <c r="N55" s="52"/>
+      <c r="O55" s="53"/>
+      <c r="P55" s="54"/>
+      <c r="Q55" s="53"/>
+      <c r="R55" s="53"/>
+      <c r="S55" s="53"/>
+      <c r="T55" s="53"/>
+      <c r="U55" s="53"/>
+      <c r="V55" s="45"/>
     </row>
     <row r="56" spans="1:22" ht="27" customHeight="1">
-      <c r="A56" s="72"/>
-      <c r="B56" s="73"/>
-      <c r="C56" s="73"/>
-      <c r="D56" s="73"/>
-      <c r="E56" s="73"/>
-      <c r="F56" s="73"/>
-      <c r="G56" s="73"/>
-      <c r="H56" s="73"/>
-      <c r="I56" s="72"/>
-      <c r="J56" s="73"/>
-      <c r="K56" s="72"/>
-      <c r="L56" s="72"/>
-      <c r="M56" s="72"/>
-      <c r="N56" s="72"/>
-      <c r="O56" s="73"/>
-      <c r="P56" s="74"/>
-      <c r="Q56" s="73"/>
-      <c r="R56" s="73"/>
-      <c r="S56" s="73"/>
-      <c r="T56" s="73"/>
-      <c r="U56" s="73"/>
-      <c r="V56" s="65"/>
+      <c r="A56" s="52"/>
+      <c r="B56" s="53"/>
+      <c r="C56" s="53"/>
+      <c r="D56" s="53"/>
+      <c r="E56" s="53"/>
+      <c r="F56" s="53"/>
+      <c r="G56" s="53"/>
+      <c r="H56" s="53"/>
+      <c r="I56" s="52"/>
+      <c r="J56" s="53"/>
+      <c r="K56" s="52"/>
+      <c r="L56" s="52"/>
+      <c r="M56" s="52"/>
+      <c r="N56" s="52"/>
+      <c r="O56" s="53"/>
+      <c r="P56" s="54"/>
+      <c r="Q56" s="53"/>
+      <c r="R56" s="53"/>
+      <c r="S56" s="53"/>
+      <c r="T56" s="53"/>
+      <c r="U56" s="53"/>
+      <c r="V56" s="45"/>
     </row>
     <row r="57" spans="1:22" ht="27" customHeight="1">
-      <c r="A57" s="72"/>
-      <c r="B57" s="73"/>
-      <c r="C57" s="73"/>
-      <c r="D57" s="73"/>
-      <c r="E57" s="73"/>
-      <c r="F57" s="73"/>
-      <c r="G57" s="73"/>
-      <c r="H57" s="73"/>
-      <c r="I57" s="72"/>
-      <c r="J57" s="73"/>
-      <c r="K57" s="72"/>
-      <c r="L57" s="72"/>
-      <c r="M57" s="72"/>
-      <c r="N57" s="72"/>
-      <c r="O57" s="73"/>
-      <c r="P57" s="74"/>
-      <c r="Q57" s="73"/>
-      <c r="R57" s="73"/>
-      <c r="S57" s="73"/>
-      <c r="T57" s="73"/>
-      <c r="U57" s="73"/>
-      <c r="V57" s="65"/>
+      <c r="A57" s="52"/>
+      <c r="B57" s="53"/>
+      <c r="C57" s="53"/>
+      <c r="D57" s="53"/>
+      <c r="E57" s="53"/>
+      <c r="F57" s="53"/>
+      <c r="G57" s="53"/>
+      <c r="H57" s="53"/>
+      <c r="I57" s="52"/>
+      <c r="J57" s="53"/>
+      <c r="K57" s="52"/>
+      <c r="L57" s="52"/>
+      <c r="M57" s="52"/>
+      <c r="N57" s="52"/>
+      <c r="O57" s="53"/>
+      <c r="P57" s="54"/>
+      <c r="Q57" s="53"/>
+      <c r="R57" s="53"/>
+      <c r="S57" s="53"/>
+      <c r="T57" s="53"/>
+      <c r="U57" s="53"/>
+      <c r="V57" s="45"/>
     </row>
     <row r="58" spans="1:22" ht="27" customHeight="1">
-      <c r="A58" s="72"/>
-      <c r="B58" s="73"/>
-      <c r="C58" s="73"/>
-      <c r="D58" s="73"/>
-      <c r="E58" s="73"/>
-      <c r="F58" s="73"/>
-      <c r="G58" s="73"/>
-      <c r="H58" s="73"/>
-      <c r="I58" s="72"/>
-      <c r="J58" s="73"/>
-      <c r="K58" s="72"/>
-      <c r="L58" s="72"/>
-      <c r="M58" s="72"/>
-      <c r="N58" s="72"/>
-      <c r="O58" s="73"/>
-      <c r="P58" s="74"/>
-      <c r="Q58" s="73"/>
-      <c r="R58" s="73"/>
-      <c r="S58" s="73"/>
-      <c r="T58" s="73"/>
-      <c r="U58" s="73"/>
-      <c r="V58" s="65"/>
+      <c r="A58" s="52"/>
+      <c r="B58" s="53"/>
+      <c r="C58" s="53"/>
+      <c r="D58" s="53"/>
+      <c r="E58" s="53"/>
+      <c r="F58" s="53"/>
+      <c r="G58" s="53"/>
+      <c r="H58" s="53"/>
+      <c r="I58" s="52"/>
+      <c r="J58" s="53"/>
+      <c r="K58" s="52"/>
+      <c r="L58" s="52"/>
+      <c r="M58" s="52"/>
+      <c r="N58" s="52"/>
+      <c r="O58" s="53"/>
+      <c r="P58" s="54"/>
+      <c r="Q58" s="53"/>
+      <c r="R58" s="53"/>
+      <c r="S58" s="53"/>
+      <c r="T58" s="53"/>
+      <c r="U58" s="53"/>
+      <c r="V58" s="45"/>
     </row>
     <row r="59" spans="1:22" ht="27" customHeight="1">
-      <c r="A59" s="72"/>
-      <c r="B59" s="73"/>
-      <c r="C59" s="73"/>
-      <c r="D59" s="73"/>
-      <c r="E59" s="73"/>
-      <c r="F59" s="73"/>
-      <c r="G59" s="73"/>
-      <c r="H59" s="73"/>
-      <c r="I59" s="72"/>
-      <c r="J59" s="73"/>
-      <c r="K59" s="72"/>
-      <c r="L59" s="72"/>
-      <c r="M59" s="72"/>
-      <c r="N59" s="72"/>
-      <c r="O59" s="73"/>
-      <c r="P59" s="74"/>
-      <c r="Q59" s="73"/>
-      <c r="R59" s="73"/>
-      <c r="S59" s="73"/>
-      <c r="T59" s="73"/>
-      <c r="U59" s="73"/>
-      <c r="V59" s="65"/>
+      <c r="A59" s="52"/>
+      <c r="B59" s="53"/>
+      <c r="C59" s="53"/>
+      <c r="D59" s="53"/>
+      <c r="E59" s="53"/>
+      <c r="F59" s="53"/>
+      <c r="G59" s="53"/>
+      <c r="H59" s="53"/>
+      <c r="I59" s="52"/>
+      <c r="J59" s="53"/>
+      <c r="K59" s="52"/>
+      <c r="L59" s="52"/>
+      <c r="M59" s="52"/>
+      <c r="N59" s="52"/>
+      <c r="O59" s="53"/>
+      <c r="P59" s="54"/>
+      <c r="Q59" s="53"/>
+      <c r="R59" s="53"/>
+      <c r="S59" s="53"/>
+      <c r="T59" s="53"/>
+      <c r="U59" s="53"/>
+      <c r="V59" s="45"/>
     </row>
     <row r="60" spans="1:22" ht="27" customHeight="1">
-      <c r="A60" s="72"/>
-      <c r="B60" s="73"/>
-      <c r="C60" s="73"/>
-      <c r="D60" s="73"/>
-      <c r="E60" s="73"/>
-      <c r="F60" s="73"/>
-      <c r="G60" s="73"/>
-      <c r="H60" s="73"/>
-      <c r="I60" s="72"/>
-      <c r="J60" s="73"/>
-      <c r="K60" s="72"/>
-      <c r="L60" s="72"/>
-      <c r="M60" s="72"/>
-      <c r="N60" s="72"/>
-      <c r="O60" s="73"/>
-      <c r="P60" s="74"/>
-      <c r="Q60" s="73"/>
-      <c r="R60" s="73"/>
-      <c r="S60" s="73"/>
-      <c r="T60" s="73"/>
-      <c r="U60" s="73"/>
-      <c r="V60" s="65"/>
+      <c r="A60" s="52"/>
+      <c r="B60" s="53"/>
+      <c r="C60" s="53"/>
+      <c r="D60" s="53"/>
+      <c r="E60" s="53"/>
+      <c r="F60" s="53"/>
+      <c r="G60" s="53"/>
+      <c r="H60" s="53"/>
+      <c r="I60" s="52"/>
+      <c r="J60" s="53"/>
+      <c r="K60" s="52"/>
+      <c r="L60" s="52"/>
+      <c r="M60" s="52"/>
+      <c r="N60" s="52"/>
+      <c r="O60" s="53"/>
+      <c r="P60" s="54"/>
+      <c r="Q60" s="53"/>
+      <c r="R60" s="53"/>
+      <c r="S60" s="53"/>
+      <c r="T60" s="53"/>
+      <c r="U60" s="53"/>
+      <c r="V60" s="45"/>
     </row>
     <row r="61" spans="1:22" ht="27" customHeight="1">
-      <c r="A61" s="72"/>
-      <c r="B61" s="73"/>
-      <c r="C61" s="73"/>
-      <c r="D61" s="73"/>
-      <c r="E61" s="73"/>
-      <c r="F61" s="73"/>
-      <c r="G61" s="73"/>
-      <c r="H61" s="73"/>
-      <c r="I61" s="72"/>
-      <c r="J61" s="73"/>
-      <c r="K61" s="72"/>
-      <c r="L61" s="72"/>
-      <c r="M61" s="72"/>
-      <c r="N61" s="72"/>
-      <c r="O61" s="73"/>
-      <c r="P61" s="74"/>
-      <c r="Q61" s="73"/>
-      <c r="R61" s="73"/>
-      <c r="S61" s="73"/>
-      <c r="T61" s="73"/>
-      <c r="U61" s="73"/>
-      <c r="V61" s="65"/>
+      <c r="A61" s="52"/>
+      <c r="B61" s="53"/>
+      <c r="C61" s="53"/>
+      <c r="D61" s="53"/>
+      <c r="E61" s="53"/>
+      <c r="F61" s="53"/>
+      <c r="G61" s="53"/>
+      <c r="H61" s="53"/>
+      <c r="I61" s="52"/>
+      <c r="J61" s="53"/>
+      <c r="K61" s="52"/>
+      <c r="L61" s="52"/>
+      <c r="M61" s="52"/>
+      <c r="N61" s="52"/>
+      <c r="O61" s="53"/>
+      <c r="P61" s="54"/>
+      <c r="Q61" s="53"/>
+      <c r="R61" s="53"/>
+      <c r="S61" s="53"/>
+      <c r="T61" s="53"/>
+      <c r="U61" s="53"/>
+      <c r="V61" s="45"/>
     </row>
     <row r="62" spans="1:22" ht="27" customHeight="1">
-      <c r="A62" s="72"/>
-      <c r="B62" s="73"/>
-      <c r="C62" s="73"/>
-      <c r="D62" s="73"/>
-      <c r="E62" s="73"/>
-      <c r="F62" s="73"/>
-      <c r="G62" s="73"/>
-      <c r="H62" s="73"/>
-      <c r="I62" s="72"/>
-      <c r="J62" s="73"/>
-      <c r="K62" s="72"/>
-      <c r="L62" s="72"/>
-      <c r="M62" s="72"/>
-      <c r="N62" s="72"/>
-      <c r="O62" s="73"/>
-      <c r="P62" s="74"/>
-      <c r="Q62" s="73"/>
-      <c r="R62" s="73"/>
-      <c r="S62" s="73"/>
-      <c r="T62" s="73"/>
-      <c r="U62" s="73"/>
-      <c r="V62" s="65"/>
+      <c r="A62" s="52"/>
+      <c r="B62" s="53"/>
+      <c r="C62" s="53"/>
+      <c r="D62" s="53"/>
+      <c r="E62" s="53"/>
+      <c r="F62" s="53"/>
+      <c r="G62" s="53"/>
+      <c r="H62" s="53"/>
+      <c r="I62" s="52"/>
+      <c r="J62" s="53"/>
+      <c r="K62" s="52"/>
+      <c r="L62" s="52"/>
+      <c r="M62" s="52"/>
+      <c r="N62" s="52"/>
+      <c r="O62" s="53"/>
+      <c r="P62" s="54"/>
+      <c r="Q62" s="53"/>
+      <c r="R62" s="53"/>
+      <c r="S62" s="53"/>
+      <c r="T62" s="53"/>
+      <c r="U62" s="53"/>
+      <c r="V62" s="45"/>
     </row>
     <row r="63" spans="1:22" ht="27" customHeight="1">
-      <c r="A63" s="72"/>
-      <c r="B63" s="73"/>
-      <c r="C63" s="73"/>
-      <c r="D63" s="73"/>
-      <c r="E63" s="73"/>
-      <c r="F63" s="73"/>
-      <c r="G63" s="73"/>
-      <c r="H63" s="73"/>
-      <c r="I63" s="72"/>
-      <c r="J63" s="73"/>
-      <c r="K63" s="72"/>
-      <c r="L63" s="72"/>
-      <c r="M63" s="72"/>
-      <c r="N63" s="72"/>
-      <c r="O63" s="73"/>
-      <c r="P63" s="74"/>
-      <c r="Q63" s="73"/>
-      <c r="R63" s="73"/>
-      <c r="S63" s="73"/>
-      <c r="T63" s="73"/>
-      <c r="U63" s="73"/>
-      <c r="V63" s="65"/>
+      <c r="A63" s="52"/>
+      <c r="B63" s="53"/>
+      <c r="C63" s="53"/>
+      <c r="D63" s="53"/>
+      <c r="E63" s="53"/>
+      <c r="F63" s="53"/>
+      <c r="G63" s="53"/>
+      <c r="H63" s="53"/>
+      <c r="I63" s="52"/>
+      <c r="J63" s="53"/>
+      <c r="K63" s="52"/>
+      <c r="L63" s="52"/>
+      <c r="M63" s="52"/>
+      <c r="N63" s="52"/>
+      <c r="O63" s="53"/>
+      <c r="P63" s="54"/>
+      <c r="Q63" s="53"/>
+      <c r="R63" s="53"/>
+      <c r="S63" s="53"/>
+      <c r="T63" s="53"/>
+      <c r="U63" s="53"/>
+      <c r="V63" s="45"/>
     </row>
     <row r="78" spans="1:1" ht="27" customHeight="1">
-      <c r="A78" s="39" t="s">
+      <c r="A78" s="19" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="79" spans="1:1" ht="27" customHeight="1">
-      <c r="A79" s="39" t="s">
+      <c r="A79" s="19" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="80" spans="1:1" ht="27" customHeight="1">
-      <c r="A80" s="39" t="s">
+      <c r="A80" s="19" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="81" spans="1:1" ht="27" customHeight="1">
-      <c r="A81" s="39" t="s">
+      <c r="A81" s="19" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="82" spans="1:1" ht="27" customHeight="1">
-      <c r="A82" s="39" t="s">
+      <c r="A82" s="19" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="83" spans="1:1" ht="27" customHeight="1">
-      <c r="A83" s="39" t="s">
+      <c r="A83" s="19" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="84" spans="1:1" ht="27" customHeight="1">
-      <c r="A84" s="39" t="s">
+      <c r="A84" s="19" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="85" spans="1:1" ht="27" customHeight="1">
-      <c r="A85" s="39" t="s">
+      <c r="A85" s="19" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="86" spans="1:1" ht="27" customHeight="1">
-      <c r="A86" s="39" t="s">
+      <c r="A86" s="19" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="87" spans="1:1" ht="27" customHeight="1">
-      <c r="A87" s="39" t="s">
+      <c r="A87" s="19" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="88" spans="1:1" ht="27" customHeight="1">
-      <c r="A88" s="39" t="s">
+      <c r="A88" s="19" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="27" customHeight="1">
-      <c r="A89" s="39" t="s">
+      <c r="A89" s="19" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="27" customHeight="1">
-      <c r="A90" s="39" t="s">
+      <c r="A90" s="19" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="91" spans="1:1" ht="27" customHeight="1">
-      <c r="A91" s="39" t="s">
+      <c r="A91" s="19" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="92" spans="1:1" ht="27" customHeight="1">
-      <c r="A92" s="39" t="s">
+      <c r="A92" s="19" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="93" spans="1:1" ht="27" customHeight="1">
-      <c r="A93" s="39" t="s">
+      <c r="A93" s="19" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="94" spans="1:1" ht="27" customHeight="1">
-      <c r="A94" s="39" t="s">
+      <c r="A94" s="19" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="95" spans="1:1" ht="27" customHeight="1">
-      <c r="A95" s="39" t="s">
+      <c r="A95" s="19" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="96" spans="1:1" ht="27" customHeight="1">
-      <c r="A96" s="39" t="s">
+      <c r="A96" s="19" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="97" spans="1:1" ht="27" customHeight="1">
-      <c r="A97" s="39" t="s">
+      <c r="A97" s="19" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="98" spans="1:1" ht="27" customHeight="1">
-      <c r="A98" s="39" t="s">
+      <c r="A98" s="19" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="99" spans="1:1" ht="27" customHeight="1">
-      <c r="A99" s="39" t="s">
+      <c r="A99" s="19" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="100" spans="1:1" ht="27" customHeight="1">
-      <c r="A100" s="39" t="s">
+      <c r="A100" s="19" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="101" spans="1:1" ht="27" customHeight="1">
-      <c r="A101" s="39" t="s">
+      <c r="A101" s="19" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="102" spans="1:1" ht="27" customHeight="1">
-      <c r="A102" s="39" t="s">
+      <c r="A102" s="19" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="103" spans="1:1" ht="27" customHeight="1">
-      <c r="A103" s="39" t="s">
+      <c r="A103" s="19" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="104" spans="1:1" ht="27" customHeight="1">
-      <c r="A104" s="39" t="s">
+      <c r="A104" s="19" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="105" spans="1:1" ht="27" customHeight="1">
-      <c r="A105" s="39" t="s">
+      <c r="A105" s="19" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="106" spans="1:1" ht="27" customHeight="1">
-      <c r="A106" s="39" t="s">
+      <c r="A106" s="19" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="107" spans="1:1" ht="27" customHeight="1">
-      <c r="A107" s="39" t="s">
+      <c r="A107" s="19" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="108" spans="1:1" ht="27" customHeight="1">
-      <c r="A108" s="39" t="s">
+      <c r="A108" s="19" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="109" spans="1:1" ht="27" customHeight="1">
-      <c r="A109" s="39" t="s">
+      <c r="A109" s="19" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="110" spans="1:1" ht="27" customHeight="1">
-      <c r="A110" s="39" t="s">
+      <c r="A110" s="19" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="111" spans="1:1" ht="27" customHeight="1">
-      <c r="A111" s="39" t="s">
+      <c r="A111" s="19" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="112" spans="1:1" ht="27" customHeight="1">
-      <c r="A112" s="39" t="s">
+      <c r="A112" s="19" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="113" spans="1:1" ht="27" customHeight="1">
-      <c r="A113" s="39" t="s">
+      <c r="A113" s="19" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="114" spans="1:1" ht="27" customHeight="1">
-      <c r="A114" s="39" t="s">
+      <c r="A114" s="19" t="s">
         <v>115</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="F1:F2"/>
     <mergeCell ref="U1:U2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="S1:S2"/>
     <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="M1:N1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="C1:C2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="O17" r:id="rId1"/>

</xml_diff>